<commit_message>
Close #23 Update product properties
</commit_message>
<xml_diff>
--- a/spec/support/data/product_import_ok.xlsx
+++ b/spec/support/data/product_import_ok.xlsx
@@ -123,10 +123,10 @@
     <t>Property Type</t>
   </si>
   <si>
-    <t>Property Material</t>
-  </si>
-  <si>
-    <t>Property Brand</t>
+    <t>Property material</t>
+  </si>
+  <si>
+    <t>Property Condition</t>
   </si>
   <si>
     <t>Image</t>
@@ -183,7 +183,7 @@
     <t>Cotton</t>
   </si>
   <si>
-    <t>Levis</t>
+    <t>Fare</t>
   </si>
   <si>
     <t>https://vtenh-dev.s3-ap-southeast-1.amazonaws.com/test/product-1.jpeg</t>
@@ -228,7 +228,7 @@
     <t>Beautiful Winter 2021 Tshirt</t>
   </si>
   <si>
-    <t>Nike</t>
+    <t>Good</t>
   </si>
   <si>
     <t>SKU</t>
@@ -365,7 +365,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -377,9 +377,13 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <u/>
       <sz val="11.0"/>
@@ -390,7 +394,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <u/>
       <sz val="11.0"/>
@@ -418,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -431,36 +434,42 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -771,10 +780,10 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
@@ -783,3143 +792,3140 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="3"/>
+      <c r="AG1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>5.0</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="R2" s="5">
+      <c r="P2" s="4"/>
+      <c r="R2" s="6">
         <v>44604.0</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3" t="s">
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>10.0</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="9">
         <v>44619.0</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="6">
         <v>44995.0</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="X3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4">
-      <c r="R4" s="8"/>
+      <c r="R4" s="10"/>
     </row>
     <row r="5">
-      <c r="R5" s="8"/>
+      <c r="R5" s="10"/>
     </row>
     <row r="6">
-      <c r="R6" s="8"/>
+      <c r="R6" s="10"/>
     </row>
     <row r="7">
-      <c r="R7" s="8"/>
+      <c r="R7" s="10"/>
     </row>
     <row r="8">
-      <c r="R8" s="8"/>
+      <c r="R8" s="10"/>
     </row>
     <row r="9">
-      <c r="R9" s="8"/>
+      <c r="R9" s="10"/>
     </row>
     <row r="10">
-      <c r="R10" s="8"/>
+      <c r="R10" s="10"/>
     </row>
     <row r="11">
-      <c r="R11" s="8"/>
+      <c r="R11" s="10"/>
     </row>
     <row r="12">
-      <c r="R12" s="8"/>
+      <c r="R12" s="10"/>
     </row>
     <row r="13">
-      <c r="R13" s="8"/>
+      <c r="R13" s="10"/>
     </row>
     <row r="14">
-      <c r="R14" s="8"/>
+      <c r="R14" s="10"/>
     </row>
     <row r="15">
-      <c r="R15" s="8"/>
+      <c r="R15" s="10"/>
     </row>
     <row r="16">
-      <c r="R16" s="8"/>
+      <c r="R16" s="10"/>
     </row>
     <row r="17">
-      <c r="R17" s="8"/>
+      <c r="R17" s="10"/>
     </row>
     <row r="18">
-      <c r="R18" s="8"/>
+      <c r="R18" s="10"/>
     </row>
     <row r="19">
-      <c r="R19" s="8"/>
+      <c r="R19" s="10"/>
     </row>
     <row r="20">
-      <c r="R20" s="8"/>
+      <c r="R20" s="10"/>
     </row>
     <row r="21">
-      <c r="R21" s="8"/>
+      <c r="R21" s="10"/>
     </row>
     <row r="22">
-      <c r="R22" s="8"/>
+      <c r="R22" s="10"/>
     </row>
     <row r="23">
-      <c r="R23" s="8"/>
+      <c r="R23" s="10"/>
     </row>
     <row r="24">
-      <c r="R24" s="8"/>
+      <c r="R24" s="10"/>
     </row>
     <row r="25">
-      <c r="R25" s="8"/>
+      <c r="R25" s="10"/>
     </row>
     <row r="26">
-      <c r="R26" s="8"/>
+      <c r="R26" s="10"/>
     </row>
     <row r="27">
-      <c r="R27" s="8"/>
+      <c r="R27" s="10"/>
     </row>
     <row r="28">
-      <c r="R28" s="8"/>
+      <c r="R28" s="10"/>
     </row>
     <row r="29">
-      <c r="R29" s="8"/>
+      <c r="R29" s="10"/>
     </row>
     <row r="30">
-      <c r="R30" s="8"/>
+      <c r="R30" s="10"/>
     </row>
     <row r="31">
-      <c r="R31" s="8"/>
+      <c r="R31" s="10"/>
     </row>
     <row r="32">
-      <c r="R32" s="8"/>
+      <c r="R32" s="10"/>
     </row>
     <row r="33">
-      <c r="R33" s="8"/>
+      <c r="R33" s="10"/>
     </row>
     <row r="34">
-      <c r="R34" s="8"/>
+      <c r="R34" s="10"/>
     </row>
     <row r="35">
-      <c r="R35" s="8"/>
+      <c r="R35" s="10"/>
     </row>
     <row r="36">
-      <c r="R36" s="8"/>
+      <c r="R36" s="10"/>
     </row>
     <row r="37">
-      <c r="R37" s="8"/>
+      <c r="R37" s="10"/>
     </row>
     <row r="38">
-      <c r="R38" s="8"/>
+      <c r="R38" s="10"/>
     </row>
     <row r="39">
-      <c r="R39" s="8"/>
+      <c r="R39" s="10"/>
     </row>
     <row r="40">
-      <c r="R40" s="8"/>
+      <c r="R40" s="10"/>
     </row>
     <row r="41">
-      <c r="R41" s="8"/>
+      <c r="R41" s="10"/>
     </row>
     <row r="42">
-      <c r="R42" s="8"/>
+      <c r="R42" s="10"/>
     </row>
     <row r="43">
-      <c r="R43" s="8"/>
+      <c r="R43" s="10"/>
     </row>
     <row r="44">
-      <c r="R44" s="8"/>
+      <c r="R44" s="10"/>
     </row>
     <row r="45">
-      <c r="R45" s="8"/>
+      <c r="R45" s="10"/>
     </row>
     <row r="46">
-      <c r="R46" s="8"/>
+      <c r="R46" s="10"/>
     </row>
     <row r="47">
-      <c r="R47" s="8"/>
+      <c r="R47" s="10"/>
     </row>
     <row r="48">
-      <c r="R48" s="8"/>
+      <c r="R48" s="10"/>
     </row>
     <row r="49">
-      <c r="R49" s="8"/>
+      <c r="R49" s="10"/>
     </row>
     <row r="50">
-      <c r="R50" s="8"/>
+      <c r="R50" s="10"/>
     </row>
     <row r="51">
-      <c r="R51" s="8"/>
+      <c r="R51" s="10"/>
     </row>
     <row r="52">
-      <c r="R52" s="8"/>
+      <c r="R52" s="10"/>
     </row>
     <row r="53">
-      <c r="R53" s="8"/>
+      <c r="R53" s="10"/>
     </row>
     <row r="54">
-      <c r="R54" s="8"/>
+      <c r="R54" s="10"/>
     </row>
     <row r="55">
-      <c r="R55" s="8"/>
+      <c r="R55" s="10"/>
     </row>
     <row r="56">
-      <c r="R56" s="8"/>
+      <c r="R56" s="10"/>
     </row>
     <row r="57">
-      <c r="R57" s="8"/>
+      <c r="R57" s="10"/>
     </row>
     <row r="58">
-      <c r="R58" s="8"/>
+      <c r="R58" s="10"/>
     </row>
     <row r="59">
-      <c r="R59" s="8"/>
+      <c r="R59" s="10"/>
     </row>
     <row r="60">
-      <c r="R60" s="8"/>
+      <c r="R60" s="10"/>
     </row>
     <row r="61">
-      <c r="R61" s="8"/>
+      <c r="R61" s="10"/>
     </row>
     <row r="62">
-      <c r="R62" s="8"/>
+      <c r="R62" s="10"/>
     </row>
     <row r="63">
-      <c r="R63" s="8"/>
+      <c r="R63" s="10"/>
     </row>
     <row r="64">
-      <c r="R64" s="8"/>
+      <c r="R64" s="10"/>
     </row>
     <row r="65">
-      <c r="R65" s="8"/>
+      <c r="R65" s="10"/>
     </row>
     <row r="66">
-      <c r="R66" s="8"/>
+      <c r="R66" s="10"/>
     </row>
     <row r="67">
-      <c r="R67" s="8"/>
+      <c r="R67" s="10"/>
     </row>
     <row r="68">
-      <c r="R68" s="8"/>
+      <c r="R68" s="10"/>
     </row>
     <row r="69">
-      <c r="R69" s="8"/>
+      <c r="R69" s="10"/>
     </row>
     <row r="70">
-      <c r="R70" s="8"/>
+      <c r="R70" s="10"/>
     </row>
     <row r="71">
-      <c r="R71" s="8"/>
+      <c r="R71" s="10"/>
     </row>
     <row r="72">
-      <c r="R72" s="8"/>
+      <c r="R72" s="10"/>
     </row>
     <row r="73">
-      <c r="R73" s="8"/>
+      <c r="R73" s="10"/>
     </row>
     <row r="74">
-      <c r="R74" s="8"/>
+      <c r="R74" s="10"/>
     </row>
     <row r="75">
-      <c r="R75" s="8"/>
+      <c r="R75" s="10"/>
     </row>
     <row r="76">
-      <c r="R76" s="8"/>
+      <c r="R76" s="10"/>
     </row>
     <row r="77">
-      <c r="R77" s="8"/>
+      <c r="R77" s="10"/>
     </row>
     <row r="78">
-      <c r="R78" s="8"/>
+      <c r="R78" s="10"/>
     </row>
     <row r="79">
-      <c r="R79" s="8"/>
+      <c r="R79" s="10"/>
     </row>
     <row r="80">
-      <c r="R80" s="8"/>
+      <c r="R80" s="10"/>
     </row>
     <row r="81">
-      <c r="R81" s="8"/>
+      <c r="R81" s="10"/>
     </row>
     <row r="82">
-      <c r="R82" s="8"/>
+      <c r="R82" s="10"/>
     </row>
     <row r="83">
-      <c r="R83" s="8"/>
+      <c r="R83" s="10"/>
     </row>
     <row r="84">
-      <c r="R84" s="8"/>
+      <c r="R84" s="10"/>
     </row>
     <row r="85">
-      <c r="R85" s="8"/>
+      <c r="R85" s="10"/>
     </row>
     <row r="86">
-      <c r="R86" s="8"/>
+      <c r="R86" s="10"/>
     </row>
     <row r="87">
-      <c r="R87" s="8"/>
+      <c r="R87" s="10"/>
     </row>
     <row r="88">
-      <c r="R88" s="8"/>
+      <c r="R88" s="10"/>
     </row>
     <row r="89">
-      <c r="R89" s="8"/>
+      <c r="R89" s="10"/>
     </row>
     <row r="90">
-      <c r="R90" s="8"/>
+      <c r="R90" s="10"/>
     </row>
     <row r="91">
-      <c r="R91" s="8"/>
+      <c r="R91" s="10"/>
     </row>
     <row r="92">
-      <c r="R92" s="8"/>
+      <c r="R92" s="10"/>
     </row>
     <row r="93">
-      <c r="R93" s="8"/>
+      <c r="R93" s="10"/>
     </row>
     <row r="94">
-      <c r="R94" s="8"/>
+      <c r="R94" s="10"/>
     </row>
     <row r="95">
-      <c r="R95" s="8"/>
+      <c r="R95" s="10"/>
     </row>
     <row r="96">
-      <c r="R96" s="8"/>
+      <c r="R96" s="10"/>
     </row>
     <row r="97">
-      <c r="R97" s="8"/>
+      <c r="R97" s="10"/>
     </row>
     <row r="98">
-      <c r="R98" s="8"/>
+      <c r="R98" s="10"/>
     </row>
     <row r="99">
-      <c r="R99" s="8"/>
+      <c r="R99" s="10"/>
     </row>
     <row r="100">
-      <c r="R100" s="8"/>
+      <c r="R100" s="10"/>
     </row>
     <row r="101">
-      <c r="R101" s="8"/>
+      <c r="R101" s="10"/>
     </row>
     <row r="102">
-      <c r="R102" s="8"/>
+      <c r="R102" s="10"/>
     </row>
     <row r="103">
-      <c r="R103" s="8"/>
+      <c r="R103" s="10"/>
     </row>
     <row r="104">
-      <c r="R104" s="8"/>
+      <c r="R104" s="10"/>
     </row>
     <row r="105">
-      <c r="R105" s="8"/>
+      <c r="R105" s="10"/>
     </row>
     <row r="106">
-      <c r="R106" s="8"/>
+      <c r="R106" s="10"/>
     </row>
     <row r="107">
-      <c r="R107" s="8"/>
+      <c r="R107" s="10"/>
     </row>
     <row r="108">
-      <c r="R108" s="8"/>
+      <c r="R108" s="10"/>
     </row>
     <row r="109">
-      <c r="R109" s="8"/>
+      <c r="R109" s="10"/>
     </row>
     <row r="110">
-      <c r="R110" s="8"/>
+      <c r="R110" s="10"/>
     </row>
     <row r="111">
-      <c r="R111" s="8"/>
+      <c r="R111" s="10"/>
     </row>
     <row r="112">
-      <c r="R112" s="8"/>
+      <c r="R112" s="10"/>
     </row>
     <row r="113">
-      <c r="R113" s="8"/>
+      <c r="R113" s="10"/>
     </row>
     <row r="114">
-      <c r="R114" s="8"/>
+      <c r="R114" s="10"/>
     </row>
     <row r="115">
-      <c r="R115" s="8"/>
+      <c r="R115" s="10"/>
     </row>
     <row r="116">
-      <c r="R116" s="8"/>
+      <c r="R116" s="10"/>
     </row>
     <row r="117">
-      <c r="R117" s="8"/>
+      <c r="R117" s="10"/>
     </row>
     <row r="118">
-      <c r="R118" s="8"/>
+      <c r="R118" s="10"/>
     </row>
     <row r="119">
-      <c r="R119" s="8"/>
+      <c r="R119" s="10"/>
     </row>
     <row r="120">
-      <c r="R120" s="8"/>
+      <c r="R120" s="10"/>
     </row>
     <row r="121">
-      <c r="R121" s="8"/>
+      <c r="R121" s="10"/>
     </row>
     <row r="122">
-      <c r="R122" s="8"/>
+      <c r="R122" s="10"/>
     </row>
     <row r="123">
-      <c r="R123" s="8"/>
+      <c r="R123" s="10"/>
     </row>
     <row r="124">
-      <c r="R124" s="8"/>
+      <c r="R124" s="10"/>
     </row>
     <row r="125">
-      <c r="R125" s="8"/>
+      <c r="R125" s="10"/>
     </row>
     <row r="126">
-      <c r="R126" s="8"/>
+      <c r="R126" s="10"/>
     </row>
     <row r="127">
-      <c r="R127" s="8"/>
+      <c r="R127" s="10"/>
     </row>
     <row r="128">
-      <c r="R128" s="8"/>
+      <c r="R128" s="10"/>
     </row>
     <row r="129">
-      <c r="R129" s="8"/>
+      <c r="R129" s="10"/>
     </row>
     <row r="130">
-      <c r="R130" s="8"/>
+      <c r="R130" s="10"/>
     </row>
     <row r="131">
-      <c r="R131" s="8"/>
+      <c r="R131" s="10"/>
     </row>
     <row r="132">
-      <c r="R132" s="8"/>
+      <c r="R132" s="10"/>
     </row>
     <row r="133">
-      <c r="R133" s="8"/>
+      <c r="R133" s="10"/>
     </row>
     <row r="134">
-      <c r="R134" s="8"/>
+      <c r="R134" s="10"/>
     </row>
     <row r="135">
-      <c r="R135" s="8"/>
+      <c r="R135" s="10"/>
     </row>
     <row r="136">
-      <c r="R136" s="8"/>
+      <c r="R136" s="10"/>
     </row>
     <row r="137">
-      <c r="R137" s="8"/>
+      <c r="R137" s="10"/>
     </row>
     <row r="138">
-      <c r="R138" s="8"/>
+      <c r="R138" s="10"/>
     </row>
     <row r="139">
-      <c r="R139" s="8"/>
+      <c r="R139" s="10"/>
     </row>
     <row r="140">
-      <c r="R140" s="8"/>
+      <c r="R140" s="10"/>
     </row>
     <row r="141">
-      <c r="R141" s="8"/>
+      <c r="R141" s="10"/>
     </row>
     <row r="142">
-      <c r="R142" s="8"/>
+      <c r="R142" s="10"/>
     </row>
     <row r="143">
-      <c r="R143" s="8"/>
+      <c r="R143" s="10"/>
     </row>
     <row r="144">
-      <c r="R144" s="8"/>
+      <c r="R144" s="10"/>
     </row>
     <row r="145">
-      <c r="R145" s="8"/>
+      <c r="R145" s="10"/>
     </row>
     <row r="146">
-      <c r="R146" s="8"/>
+      <c r="R146" s="10"/>
     </row>
     <row r="147">
-      <c r="R147" s="8"/>
+      <c r="R147" s="10"/>
     </row>
     <row r="148">
-      <c r="R148" s="8"/>
+      <c r="R148" s="10"/>
     </row>
     <row r="149">
-      <c r="R149" s="8"/>
+      <c r="R149" s="10"/>
     </row>
     <row r="150">
-      <c r="R150" s="8"/>
+      <c r="R150" s="10"/>
     </row>
     <row r="151">
-      <c r="R151" s="8"/>
+      <c r="R151" s="10"/>
     </row>
     <row r="152">
-      <c r="R152" s="8"/>
+      <c r="R152" s="10"/>
     </row>
     <row r="153">
-      <c r="R153" s="8"/>
+      <c r="R153" s="10"/>
     </row>
     <row r="154">
-      <c r="R154" s="8"/>
+      <c r="R154" s="10"/>
     </row>
     <row r="155">
-      <c r="R155" s="8"/>
+      <c r="R155" s="10"/>
     </row>
     <row r="156">
-      <c r="R156" s="8"/>
+      <c r="R156" s="10"/>
     </row>
     <row r="157">
-      <c r="R157" s="8"/>
+      <c r="R157" s="10"/>
     </row>
     <row r="158">
-      <c r="R158" s="8"/>
+      <c r="R158" s="10"/>
     </row>
     <row r="159">
-      <c r="R159" s="8"/>
+      <c r="R159" s="10"/>
     </row>
     <row r="160">
-      <c r="R160" s="8"/>
+      <c r="R160" s="10"/>
     </row>
     <row r="161">
-      <c r="R161" s="8"/>
+      <c r="R161" s="10"/>
     </row>
     <row r="162">
-      <c r="R162" s="8"/>
+      <c r="R162" s="10"/>
     </row>
     <row r="163">
-      <c r="R163" s="8"/>
+      <c r="R163" s="10"/>
     </row>
     <row r="164">
-      <c r="R164" s="8"/>
+      <c r="R164" s="10"/>
     </row>
     <row r="165">
-      <c r="R165" s="8"/>
+      <c r="R165" s="10"/>
     </row>
     <row r="166">
-      <c r="R166" s="8"/>
+      <c r="R166" s="10"/>
     </row>
     <row r="167">
-      <c r="R167" s="8"/>
+      <c r="R167" s="10"/>
     </row>
     <row r="168">
-      <c r="R168" s="8"/>
+      <c r="R168" s="10"/>
     </row>
     <row r="169">
-      <c r="R169" s="8"/>
+      <c r="R169" s="10"/>
     </row>
     <row r="170">
-      <c r="R170" s="8"/>
+      <c r="R170" s="10"/>
     </row>
     <row r="171">
-      <c r="R171" s="8"/>
+      <c r="R171" s="10"/>
     </row>
     <row r="172">
-      <c r="R172" s="8"/>
+      <c r="R172" s="10"/>
     </row>
     <row r="173">
-      <c r="R173" s="8"/>
+      <c r="R173" s="10"/>
     </row>
     <row r="174">
-      <c r="R174" s="8"/>
+      <c r="R174" s="10"/>
     </row>
     <row r="175">
-      <c r="R175" s="8"/>
+      <c r="R175" s="10"/>
     </row>
     <row r="176">
-      <c r="R176" s="8"/>
+      <c r="R176" s="10"/>
     </row>
     <row r="177">
-      <c r="R177" s="8"/>
+      <c r="R177" s="10"/>
     </row>
     <row r="178">
-      <c r="R178" s="8"/>
+      <c r="R178" s="10"/>
     </row>
     <row r="179">
-      <c r="R179" s="8"/>
+      <c r="R179" s="10"/>
     </row>
     <row r="180">
-      <c r="R180" s="8"/>
+      <c r="R180" s="10"/>
     </row>
     <row r="181">
-      <c r="R181" s="8"/>
+      <c r="R181" s="10"/>
     </row>
     <row r="182">
-      <c r="R182" s="8"/>
+      <c r="R182" s="10"/>
     </row>
     <row r="183">
-      <c r="R183" s="8"/>
+      <c r="R183" s="10"/>
     </row>
     <row r="184">
-      <c r="R184" s="8"/>
+      <c r="R184" s="10"/>
     </row>
     <row r="185">
-      <c r="R185" s="8"/>
+      <c r="R185" s="10"/>
     </row>
     <row r="186">
-      <c r="R186" s="8"/>
+      <c r="R186" s="10"/>
     </row>
     <row r="187">
-      <c r="R187" s="8"/>
+      <c r="R187" s="10"/>
     </row>
     <row r="188">
-      <c r="R188" s="8"/>
+      <c r="R188" s="10"/>
     </row>
     <row r="189">
-      <c r="R189" s="8"/>
+      <c r="R189" s="10"/>
     </row>
     <row r="190">
-      <c r="R190" s="8"/>
+      <c r="R190" s="10"/>
     </row>
     <row r="191">
-      <c r="R191" s="8"/>
+      <c r="R191" s="10"/>
     </row>
     <row r="192">
-      <c r="R192" s="8"/>
+      <c r="R192" s="10"/>
     </row>
     <row r="193">
-      <c r="R193" s="8"/>
+      <c r="R193" s="10"/>
     </row>
     <row r="194">
-      <c r="R194" s="8"/>
+      <c r="R194" s="10"/>
     </row>
     <row r="195">
-      <c r="R195" s="8"/>
+      <c r="R195" s="10"/>
     </row>
     <row r="196">
-      <c r="R196" s="8"/>
+      <c r="R196" s="10"/>
     </row>
     <row r="197">
-      <c r="R197" s="8"/>
+      <c r="R197" s="10"/>
     </row>
     <row r="198">
-      <c r="R198" s="8"/>
+      <c r="R198" s="10"/>
     </row>
     <row r="199">
-      <c r="R199" s="8"/>
+      <c r="R199" s="10"/>
     </row>
     <row r="200">
-      <c r="R200" s="8"/>
+      <c r="R200" s="10"/>
     </row>
     <row r="201">
-      <c r="R201" s="8"/>
+      <c r="R201" s="10"/>
     </row>
     <row r="202">
-      <c r="R202" s="8"/>
+      <c r="R202" s="10"/>
     </row>
     <row r="203">
-      <c r="R203" s="8"/>
+      <c r="R203" s="10"/>
     </row>
     <row r="204">
-      <c r="R204" s="8"/>
+      <c r="R204" s="10"/>
     </row>
     <row r="205">
-      <c r="R205" s="8"/>
+      <c r="R205" s="10"/>
     </row>
     <row r="206">
-      <c r="R206" s="8"/>
+      <c r="R206" s="10"/>
     </row>
     <row r="207">
-      <c r="R207" s="8"/>
+      <c r="R207" s="10"/>
     </row>
     <row r="208">
-      <c r="R208" s="8"/>
+      <c r="R208" s="10"/>
     </row>
     <row r="209">
-      <c r="R209" s="8"/>
+      <c r="R209" s="10"/>
     </row>
     <row r="210">
-      <c r="R210" s="8"/>
+      <c r="R210" s="10"/>
     </row>
     <row r="211">
-      <c r="R211" s="8"/>
+      <c r="R211" s="10"/>
     </row>
     <row r="212">
-      <c r="R212" s="8"/>
+      <c r="R212" s="10"/>
     </row>
     <row r="213">
-      <c r="R213" s="8"/>
+      <c r="R213" s="10"/>
     </row>
     <row r="214">
-      <c r="R214" s="8"/>
+      <c r="R214" s="10"/>
     </row>
     <row r="215">
-      <c r="R215" s="8"/>
+      <c r="R215" s="10"/>
     </row>
     <row r="216">
-      <c r="R216" s="8"/>
+      <c r="R216" s="10"/>
     </row>
     <row r="217">
-      <c r="R217" s="8"/>
+      <c r="R217" s="10"/>
     </row>
     <row r="218">
-      <c r="R218" s="8"/>
+      <c r="R218" s="10"/>
     </row>
     <row r="219">
-      <c r="R219" s="8"/>
+      <c r="R219" s="10"/>
     </row>
     <row r="220">
-      <c r="R220" s="8"/>
+      <c r="R220" s="10"/>
     </row>
     <row r="221">
-      <c r="R221" s="8"/>
+      <c r="R221" s="10"/>
     </row>
     <row r="222">
-      <c r="R222" s="8"/>
+      <c r="R222" s="10"/>
     </row>
     <row r="223">
-      <c r="R223" s="8"/>
+      <c r="R223" s="10"/>
     </row>
     <row r="224">
-      <c r="R224" s="8"/>
+      <c r="R224" s="10"/>
     </row>
     <row r="225">
-      <c r="R225" s="8"/>
+      <c r="R225" s="10"/>
     </row>
     <row r="226">
-      <c r="R226" s="8"/>
+      <c r="R226" s="10"/>
     </row>
     <row r="227">
-      <c r="R227" s="8"/>
+      <c r="R227" s="10"/>
     </row>
     <row r="228">
-      <c r="R228" s="8"/>
+      <c r="R228" s="10"/>
     </row>
     <row r="229">
-      <c r="R229" s="8"/>
+      <c r="R229" s="10"/>
     </row>
     <row r="230">
-      <c r="R230" s="8"/>
+      <c r="R230" s="10"/>
     </row>
     <row r="231">
-      <c r="R231" s="8"/>
+      <c r="R231" s="10"/>
     </row>
     <row r="232">
-      <c r="R232" s="8"/>
+      <c r="R232" s="10"/>
     </row>
     <row r="233">
-      <c r="R233" s="8"/>
+      <c r="R233" s="10"/>
     </row>
     <row r="234">
-      <c r="R234" s="8"/>
+      <c r="R234" s="10"/>
     </row>
     <row r="235">
-      <c r="R235" s="8"/>
+      <c r="R235" s="10"/>
     </row>
     <row r="236">
-      <c r="R236" s="8"/>
+      <c r="R236" s="10"/>
     </row>
     <row r="237">
-      <c r="R237" s="8"/>
+      <c r="R237" s="10"/>
     </row>
     <row r="238">
-      <c r="R238" s="8"/>
+      <c r="R238" s="10"/>
     </row>
     <row r="239">
-      <c r="R239" s="8"/>
+      <c r="R239" s="10"/>
     </row>
     <row r="240">
-      <c r="R240" s="8"/>
+      <c r="R240" s="10"/>
     </row>
     <row r="241">
-      <c r="R241" s="8"/>
+      <c r="R241" s="10"/>
     </row>
     <row r="242">
-      <c r="R242" s="8"/>
+      <c r="R242" s="10"/>
     </row>
     <row r="243">
-      <c r="R243" s="8"/>
+      <c r="R243" s="10"/>
     </row>
     <row r="244">
-      <c r="R244" s="8"/>
+      <c r="R244" s="10"/>
     </row>
     <row r="245">
-      <c r="R245" s="8"/>
+      <c r="R245" s="10"/>
     </row>
     <row r="246">
-      <c r="R246" s="8"/>
+      <c r="R246" s="10"/>
     </row>
     <row r="247">
-      <c r="R247" s="8"/>
+      <c r="R247" s="10"/>
     </row>
     <row r="248">
-      <c r="R248" s="8"/>
+      <c r="R248" s="10"/>
     </row>
     <row r="249">
-      <c r="R249" s="8"/>
+      <c r="R249" s="10"/>
     </row>
     <row r="250">
-      <c r="R250" s="8"/>
+      <c r="R250" s="10"/>
     </row>
     <row r="251">
-      <c r="R251" s="8"/>
+      <c r="R251" s="10"/>
     </row>
     <row r="252">
-      <c r="R252" s="8"/>
+      <c r="R252" s="10"/>
     </row>
     <row r="253">
-      <c r="R253" s="8"/>
+      <c r="R253" s="10"/>
     </row>
     <row r="254">
-      <c r="R254" s="8"/>
+      <c r="R254" s="10"/>
     </row>
     <row r="255">
-      <c r="R255" s="8"/>
+      <c r="R255" s="10"/>
     </row>
     <row r="256">
-      <c r="R256" s="8"/>
+      <c r="R256" s="10"/>
     </row>
     <row r="257">
-      <c r="R257" s="8"/>
+      <c r="R257" s="10"/>
     </row>
     <row r="258">
-      <c r="R258" s="8"/>
+      <c r="R258" s="10"/>
     </row>
     <row r="259">
-      <c r="R259" s="8"/>
+      <c r="R259" s="10"/>
     </row>
     <row r="260">
-      <c r="R260" s="8"/>
+      <c r="R260" s="10"/>
     </row>
     <row r="261">
-      <c r="R261" s="8"/>
+      <c r="R261" s="10"/>
     </row>
     <row r="262">
-      <c r="R262" s="8"/>
+      <c r="R262" s="10"/>
     </row>
     <row r="263">
-      <c r="R263" s="8"/>
+      <c r="R263" s="10"/>
     </row>
     <row r="264">
-      <c r="R264" s="8"/>
+      <c r="R264" s="10"/>
     </row>
     <row r="265">
-      <c r="R265" s="8"/>
+      <c r="R265" s="10"/>
     </row>
     <row r="266">
-      <c r="R266" s="8"/>
+      <c r="R266" s="10"/>
     </row>
     <row r="267">
-      <c r="R267" s="8"/>
+      <c r="R267" s="10"/>
     </row>
     <row r="268">
-      <c r="R268" s="8"/>
+      <c r="R268" s="10"/>
     </row>
     <row r="269">
-      <c r="R269" s="8"/>
+      <c r="R269" s="10"/>
     </row>
     <row r="270">
-      <c r="R270" s="8"/>
+      <c r="R270" s="10"/>
     </row>
     <row r="271">
-      <c r="R271" s="8"/>
+      <c r="R271" s="10"/>
     </row>
     <row r="272">
-      <c r="R272" s="8"/>
+      <c r="R272" s="10"/>
     </row>
     <row r="273">
-      <c r="R273" s="8"/>
+      <c r="R273" s="10"/>
     </row>
     <row r="274">
-      <c r="R274" s="8"/>
+      <c r="R274" s="10"/>
     </row>
     <row r="275">
-      <c r="R275" s="8"/>
+      <c r="R275" s="10"/>
     </row>
     <row r="276">
-      <c r="R276" s="8"/>
+      <c r="R276" s="10"/>
     </row>
     <row r="277">
-      <c r="R277" s="8"/>
+      <c r="R277" s="10"/>
     </row>
     <row r="278">
-      <c r="R278" s="8"/>
+      <c r="R278" s="10"/>
     </row>
     <row r="279">
-      <c r="R279" s="8"/>
+      <c r="R279" s="10"/>
     </row>
     <row r="280">
-      <c r="R280" s="8"/>
+      <c r="R280" s="10"/>
     </row>
     <row r="281">
-      <c r="R281" s="8"/>
+      <c r="R281" s="10"/>
     </row>
     <row r="282">
-      <c r="R282" s="8"/>
+      <c r="R282" s="10"/>
     </row>
     <row r="283">
-      <c r="R283" s="8"/>
+      <c r="R283" s="10"/>
     </row>
     <row r="284">
-      <c r="R284" s="8"/>
+      <c r="R284" s="10"/>
     </row>
     <row r="285">
-      <c r="R285" s="8"/>
+      <c r="R285" s="10"/>
     </row>
     <row r="286">
-      <c r="R286" s="8"/>
+      <c r="R286" s="10"/>
     </row>
     <row r="287">
-      <c r="R287" s="8"/>
+      <c r="R287" s="10"/>
     </row>
     <row r="288">
-      <c r="R288" s="8"/>
+      <c r="R288" s="10"/>
     </row>
     <row r="289">
-      <c r="R289" s="8"/>
+      <c r="R289" s="10"/>
     </row>
     <row r="290">
-      <c r="R290" s="8"/>
+      <c r="R290" s="10"/>
     </row>
     <row r="291">
-      <c r="R291" s="8"/>
+      <c r="R291" s="10"/>
     </row>
     <row r="292">
-      <c r="R292" s="8"/>
+      <c r="R292" s="10"/>
     </row>
     <row r="293">
-      <c r="R293" s="8"/>
+      <c r="R293" s="10"/>
     </row>
     <row r="294">
-      <c r="R294" s="8"/>
+      <c r="R294" s="10"/>
     </row>
     <row r="295">
-      <c r="R295" s="8"/>
+      <c r="R295" s="10"/>
     </row>
     <row r="296">
-      <c r="R296" s="8"/>
+      <c r="R296" s="10"/>
     </row>
     <row r="297">
-      <c r="R297" s="8"/>
+      <c r="R297" s="10"/>
     </row>
     <row r="298">
-      <c r="R298" s="8"/>
+      <c r="R298" s="10"/>
     </row>
     <row r="299">
-      <c r="R299" s="8"/>
+      <c r="R299" s="10"/>
     </row>
     <row r="300">
-      <c r="R300" s="8"/>
+      <c r="R300" s="10"/>
     </row>
     <row r="301">
-      <c r="R301" s="8"/>
+      <c r="R301" s="10"/>
     </row>
     <row r="302">
-      <c r="R302" s="8"/>
+      <c r="R302" s="10"/>
     </row>
     <row r="303">
-      <c r="R303" s="8"/>
+      <c r="R303" s="10"/>
     </row>
     <row r="304">
-      <c r="R304" s="8"/>
+      <c r="R304" s="10"/>
     </row>
     <row r="305">
-      <c r="R305" s="8"/>
+      <c r="R305" s="10"/>
     </row>
     <row r="306">
-      <c r="R306" s="8"/>
+      <c r="R306" s="10"/>
     </row>
     <row r="307">
-      <c r="R307" s="8"/>
+      <c r="R307" s="10"/>
     </row>
     <row r="308">
-      <c r="R308" s="8"/>
+      <c r="R308" s="10"/>
     </row>
     <row r="309">
-      <c r="R309" s="8"/>
+      <c r="R309" s="10"/>
     </row>
     <row r="310">
-      <c r="R310" s="8"/>
+      <c r="R310" s="10"/>
     </row>
     <row r="311">
-      <c r="R311" s="8"/>
+      <c r="R311" s="10"/>
     </row>
     <row r="312">
-      <c r="R312" s="8"/>
+      <c r="R312" s="10"/>
     </row>
     <row r="313">
-      <c r="R313" s="8"/>
+      <c r="R313" s="10"/>
     </row>
     <row r="314">
-      <c r="R314" s="8"/>
+      <c r="R314" s="10"/>
     </row>
     <row r="315">
-      <c r="R315" s="8"/>
+      <c r="R315" s="10"/>
     </row>
     <row r="316">
-      <c r="R316" s="8"/>
+      <c r="R316" s="10"/>
     </row>
     <row r="317">
-      <c r="R317" s="8"/>
+      <c r="R317" s="10"/>
     </row>
     <row r="318">
-      <c r="R318" s="8"/>
+      <c r="R318" s="10"/>
     </row>
     <row r="319">
-      <c r="R319" s="8"/>
+      <c r="R319" s="10"/>
     </row>
     <row r="320">
-      <c r="R320" s="8"/>
+      <c r="R320" s="10"/>
     </row>
     <row r="321">
-      <c r="R321" s="8"/>
+      <c r="R321" s="10"/>
     </row>
     <row r="322">
-      <c r="R322" s="8"/>
+      <c r="R322" s="10"/>
     </row>
     <row r="323">
-      <c r="R323" s="8"/>
+      <c r="R323" s="10"/>
     </row>
     <row r="324">
-      <c r="R324" s="8"/>
+      <c r="R324" s="10"/>
     </row>
     <row r="325">
-      <c r="R325" s="8"/>
+      <c r="R325" s="10"/>
     </row>
     <row r="326">
-      <c r="R326" s="8"/>
+      <c r="R326" s="10"/>
     </row>
     <row r="327">
-      <c r="R327" s="8"/>
+      <c r="R327" s="10"/>
     </row>
     <row r="328">
-      <c r="R328" s="8"/>
+      <c r="R328" s="10"/>
     </row>
     <row r="329">
-      <c r="R329" s="8"/>
+      <c r="R329" s="10"/>
     </row>
     <row r="330">
-      <c r="R330" s="8"/>
+      <c r="R330" s="10"/>
     </row>
     <row r="331">
-      <c r="R331" s="8"/>
+      <c r="R331" s="10"/>
     </row>
     <row r="332">
-      <c r="R332" s="8"/>
+      <c r="R332" s="10"/>
     </row>
     <row r="333">
-      <c r="R333" s="8"/>
+      <c r="R333" s="10"/>
     </row>
     <row r="334">
-      <c r="R334" s="8"/>
+      <c r="R334" s="10"/>
     </row>
     <row r="335">
-      <c r="R335" s="8"/>
+      <c r="R335" s="10"/>
     </row>
     <row r="336">
-      <c r="R336" s="8"/>
+      <c r="R336" s="10"/>
     </row>
     <row r="337">
-      <c r="R337" s="8"/>
+      <c r="R337" s="10"/>
     </row>
     <row r="338">
-      <c r="R338" s="8"/>
+      <c r="R338" s="10"/>
     </row>
     <row r="339">
-      <c r="R339" s="8"/>
+      <c r="R339" s="10"/>
     </row>
     <row r="340">
-      <c r="R340" s="8"/>
+      <c r="R340" s="10"/>
     </row>
     <row r="341">
-      <c r="R341" s="8"/>
+      <c r="R341" s="10"/>
     </row>
     <row r="342">
-      <c r="R342" s="8"/>
+      <c r="R342" s="10"/>
     </row>
     <row r="343">
-      <c r="R343" s="8"/>
+      <c r="R343" s="10"/>
     </row>
     <row r="344">
-      <c r="R344" s="8"/>
+      <c r="R344" s="10"/>
     </row>
     <row r="345">
-      <c r="R345" s="8"/>
+      <c r="R345" s="10"/>
     </row>
     <row r="346">
-      <c r="R346" s="8"/>
+      <c r="R346" s="10"/>
     </row>
     <row r="347">
-      <c r="R347" s="8"/>
+      <c r="R347" s="10"/>
     </row>
     <row r="348">
-      <c r="R348" s="8"/>
+      <c r="R348" s="10"/>
     </row>
     <row r="349">
-      <c r="R349" s="8"/>
+      <c r="R349" s="10"/>
     </row>
     <row r="350">
-      <c r="R350" s="8"/>
+      <c r="R350" s="10"/>
     </row>
     <row r="351">
-      <c r="R351" s="8"/>
+      <c r="R351" s="10"/>
     </row>
     <row r="352">
-      <c r="R352" s="8"/>
+      <c r="R352" s="10"/>
     </row>
     <row r="353">
-      <c r="R353" s="8"/>
+      <c r="R353" s="10"/>
     </row>
     <row r="354">
-      <c r="R354" s="8"/>
+      <c r="R354" s="10"/>
     </row>
     <row r="355">
-      <c r="R355" s="8"/>
+      <c r="R355" s="10"/>
     </row>
     <row r="356">
-      <c r="R356" s="8"/>
+      <c r="R356" s="10"/>
     </row>
     <row r="357">
-      <c r="R357" s="8"/>
+      <c r="R357" s="10"/>
     </row>
     <row r="358">
-      <c r="R358" s="8"/>
+      <c r="R358" s="10"/>
     </row>
     <row r="359">
-      <c r="R359" s="8"/>
+      <c r="R359" s="10"/>
     </row>
     <row r="360">
-      <c r="R360" s="8"/>
+      <c r="R360" s="10"/>
     </row>
     <row r="361">
-      <c r="R361" s="8"/>
+      <c r="R361" s="10"/>
     </row>
     <row r="362">
-      <c r="R362" s="8"/>
+      <c r="R362" s="10"/>
     </row>
     <row r="363">
-      <c r="R363" s="8"/>
+      <c r="R363" s="10"/>
     </row>
     <row r="364">
-      <c r="R364" s="8"/>
+      <c r="R364" s="10"/>
     </row>
     <row r="365">
-      <c r="R365" s="8"/>
+      <c r="R365" s="10"/>
     </row>
     <row r="366">
-      <c r="R366" s="8"/>
+      <c r="R366" s="10"/>
     </row>
     <row r="367">
-      <c r="R367" s="8"/>
+      <c r="R367" s="10"/>
     </row>
     <row r="368">
-      <c r="R368" s="8"/>
+      <c r="R368" s="10"/>
     </row>
     <row r="369">
-      <c r="R369" s="8"/>
+      <c r="R369" s="10"/>
     </row>
     <row r="370">
-      <c r="R370" s="8"/>
+      <c r="R370" s="10"/>
     </row>
     <row r="371">
-      <c r="R371" s="8"/>
+      <c r="R371" s="10"/>
     </row>
     <row r="372">
-      <c r="R372" s="8"/>
+      <c r="R372" s="10"/>
     </row>
     <row r="373">
-      <c r="R373" s="8"/>
+      <c r="R373" s="10"/>
     </row>
     <row r="374">
-      <c r="R374" s="8"/>
+      <c r="R374" s="10"/>
     </row>
     <row r="375">
-      <c r="R375" s="8"/>
+      <c r="R375" s="10"/>
     </row>
     <row r="376">
-      <c r="R376" s="8"/>
+      <c r="R376" s="10"/>
     </row>
     <row r="377">
-      <c r="R377" s="8"/>
+      <c r="R377" s="10"/>
     </row>
     <row r="378">
-      <c r="R378" s="8"/>
+      <c r="R378" s="10"/>
     </row>
     <row r="379">
-      <c r="R379" s="8"/>
+      <c r="R379" s="10"/>
     </row>
     <row r="380">
-      <c r="R380" s="8"/>
+      <c r="R380" s="10"/>
     </row>
     <row r="381">
-      <c r="R381" s="8"/>
+      <c r="R381" s="10"/>
     </row>
     <row r="382">
-      <c r="R382" s="8"/>
+      <c r="R382" s="10"/>
     </row>
     <row r="383">
-      <c r="R383" s="8"/>
+      <c r="R383" s="10"/>
     </row>
     <row r="384">
-      <c r="R384" s="8"/>
+      <c r="R384" s="10"/>
     </row>
     <row r="385">
-      <c r="R385" s="8"/>
+      <c r="R385" s="10"/>
     </row>
     <row r="386">
-      <c r="R386" s="8"/>
+      <c r="R386" s="10"/>
     </row>
     <row r="387">
-      <c r="R387" s="8"/>
+      <c r="R387" s="10"/>
     </row>
     <row r="388">
-      <c r="R388" s="8"/>
+      <c r="R388" s="10"/>
     </row>
     <row r="389">
-      <c r="R389" s="8"/>
+      <c r="R389" s="10"/>
     </row>
     <row r="390">
-      <c r="R390" s="8"/>
+      <c r="R390" s="10"/>
     </row>
     <row r="391">
-      <c r="R391" s="8"/>
+      <c r="R391" s="10"/>
     </row>
     <row r="392">
-      <c r="R392" s="8"/>
+      <c r="R392" s="10"/>
     </row>
     <row r="393">
-      <c r="R393" s="8"/>
+      <c r="R393" s="10"/>
     </row>
     <row r="394">
-      <c r="R394" s="8"/>
+      <c r="R394" s="10"/>
     </row>
     <row r="395">
-      <c r="R395" s="8"/>
+      <c r="R395" s="10"/>
     </row>
     <row r="396">
-      <c r="R396" s="8"/>
+      <c r="R396" s="10"/>
     </row>
     <row r="397">
-      <c r="R397" s="8"/>
+      <c r="R397" s="10"/>
     </row>
     <row r="398">
-      <c r="R398" s="8"/>
+      <c r="R398" s="10"/>
     </row>
     <row r="399">
-      <c r="R399" s="8"/>
+      <c r="R399" s="10"/>
     </row>
     <row r="400">
-      <c r="R400" s="8"/>
+      <c r="R400" s="10"/>
     </row>
     <row r="401">
-      <c r="R401" s="8"/>
+      <c r="R401" s="10"/>
     </row>
     <row r="402">
-      <c r="R402" s="8"/>
+      <c r="R402" s="10"/>
     </row>
     <row r="403">
-      <c r="R403" s="8"/>
+      <c r="R403" s="10"/>
     </row>
     <row r="404">
-      <c r="R404" s="8"/>
+      <c r="R404" s="10"/>
     </row>
     <row r="405">
-      <c r="R405" s="8"/>
+      <c r="R405" s="10"/>
     </row>
     <row r="406">
-      <c r="R406" s="8"/>
+      <c r="R406" s="10"/>
     </row>
     <row r="407">
-      <c r="R407" s="8"/>
+      <c r="R407" s="10"/>
     </row>
     <row r="408">
-      <c r="R408" s="8"/>
+      <c r="R408" s="10"/>
     </row>
     <row r="409">
-      <c r="R409" s="8"/>
+      <c r="R409" s="10"/>
     </row>
     <row r="410">
-      <c r="R410" s="8"/>
+      <c r="R410" s="10"/>
     </row>
     <row r="411">
-      <c r="R411" s="8"/>
+      <c r="R411" s="10"/>
     </row>
     <row r="412">
-      <c r="R412" s="8"/>
+      <c r="R412" s="10"/>
     </row>
     <row r="413">
-      <c r="R413" s="8"/>
+      <c r="R413" s="10"/>
     </row>
     <row r="414">
-      <c r="R414" s="8"/>
+      <c r="R414" s="10"/>
     </row>
     <row r="415">
-      <c r="R415" s="8"/>
+      <c r="R415" s="10"/>
     </row>
     <row r="416">
-      <c r="R416" s="8"/>
+      <c r="R416" s="10"/>
     </row>
     <row r="417">
-      <c r="R417" s="8"/>
+      <c r="R417" s="10"/>
     </row>
     <row r="418">
-      <c r="R418" s="8"/>
+      <c r="R418" s="10"/>
     </row>
     <row r="419">
-      <c r="R419" s="8"/>
+      <c r="R419" s="10"/>
     </row>
     <row r="420">
-      <c r="R420" s="8"/>
+      <c r="R420" s="10"/>
     </row>
     <row r="421">
-      <c r="R421" s="8"/>
+      <c r="R421" s="10"/>
     </row>
     <row r="422">
-      <c r="R422" s="8"/>
+      <c r="R422" s="10"/>
     </row>
     <row r="423">
-      <c r="R423" s="8"/>
+      <c r="R423" s="10"/>
     </row>
     <row r="424">
-      <c r="R424" s="8"/>
+      <c r="R424" s="10"/>
     </row>
     <row r="425">
-      <c r="R425" s="8"/>
+      <c r="R425" s="10"/>
     </row>
     <row r="426">
-      <c r="R426" s="8"/>
+      <c r="R426" s="10"/>
     </row>
     <row r="427">
-      <c r="R427" s="8"/>
+      <c r="R427" s="10"/>
     </row>
     <row r="428">
-      <c r="R428" s="8"/>
+      <c r="R428" s="10"/>
     </row>
     <row r="429">
-      <c r="R429" s="8"/>
+      <c r="R429" s="10"/>
     </row>
     <row r="430">
-      <c r="R430" s="8"/>
+      <c r="R430" s="10"/>
     </row>
     <row r="431">
-      <c r="R431" s="8"/>
+      <c r="R431" s="10"/>
     </row>
     <row r="432">
-      <c r="R432" s="8"/>
+      <c r="R432" s="10"/>
     </row>
     <row r="433">
-      <c r="R433" s="8"/>
+      <c r="R433" s="10"/>
     </row>
     <row r="434">
-      <c r="R434" s="8"/>
+      <c r="R434" s="10"/>
     </row>
     <row r="435">
-      <c r="R435" s="8"/>
+      <c r="R435" s="10"/>
     </row>
     <row r="436">
-      <c r="R436" s="8"/>
+      <c r="R436" s="10"/>
     </row>
     <row r="437">
-      <c r="R437" s="8"/>
+      <c r="R437" s="10"/>
     </row>
     <row r="438">
-      <c r="R438" s="8"/>
+      <c r="R438" s="10"/>
     </row>
     <row r="439">
-      <c r="R439" s="8"/>
+      <c r="R439" s="10"/>
     </row>
     <row r="440">
-      <c r="R440" s="8"/>
+      <c r="R440" s="10"/>
     </row>
     <row r="441">
-      <c r="R441" s="8"/>
+      <c r="R441" s="10"/>
     </row>
     <row r="442">
-      <c r="R442" s="8"/>
+      <c r="R442" s="10"/>
     </row>
     <row r="443">
-      <c r="R443" s="8"/>
+      <c r="R443" s="10"/>
     </row>
     <row r="444">
-      <c r="R444" s="8"/>
+      <c r="R444" s="10"/>
     </row>
     <row r="445">
-      <c r="R445" s="8"/>
+      <c r="R445" s="10"/>
     </row>
     <row r="446">
-      <c r="R446" s="8"/>
+      <c r="R446" s="10"/>
     </row>
     <row r="447">
-      <c r="R447" s="8"/>
+      <c r="R447" s="10"/>
     </row>
     <row r="448">
-      <c r="R448" s="8"/>
+      <c r="R448" s="10"/>
     </row>
     <row r="449">
-      <c r="R449" s="8"/>
+      <c r="R449" s="10"/>
     </row>
     <row r="450">
-      <c r="R450" s="8"/>
+      <c r="R450" s="10"/>
     </row>
     <row r="451">
-      <c r="R451" s="8"/>
+      <c r="R451" s="10"/>
     </row>
     <row r="452">
-      <c r="R452" s="8"/>
+      <c r="R452" s="10"/>
     </row>
     <row r="453">
-      <c r="R453" s="8"/>
+      <c r="R453" s="10"/>
     </row>
     <row r="454">
-      <c r="R454" s="8"/>
+      <c r="R454" s="10"/>
     </row>
     <row r="455">
-      <c r="R455" s="8"/>
+      <c r="R455" s="10"/>
     </row>
     <row r="456">
-      <c r="R456" s="8"/>
+      <c r="R456" s="10"/>
     </row>
     <row r="457">
-      <c r="R457" s="8"/>
+      <c r="R457" s="10"/>
     </row>
     <row r="458">
-      <c r="R458" s="8"/>
+      <c r="R458" s="10"/>
     </row>
     <row r="459">
-      <c r="R459" s="8"/>
+      <c r="R459" s="10"/>
     </row>
     <row r="460">
-      <c r="R460" s="8"/>
+      <c r="R460" s="10"/>
     </row>
     <row r="461">
-      <c r="R461" s="8"/>
+      <c r="R461" s="10"/>
     </row>
     <row r="462">
-      <c r="R462" s="8"/>
+      <c r="R462" s="10"/>
     </row>
     <row r="463">
-      <c r="R463" s="8"/>
+      <c r="R463" s="10"/>
     </row>
     <row r="464">
-      <c r="R464" s="8"/>
+      <c r="R464" s="10"/>
     </row>
     <row r="465">
-      <c r="R465" s="8"/>
+      <c r="R465" s="10"/>
     </row>
     <row r="466">
-      <c r="R466" s="8"/>
+      <c r="R466" s="10"/>
     </row>
     <row r="467">
-      <c r="R467" s="8"/>
+      <c r="R467" s="10"/>
     </row>
     <row r="468">
-      <c r="R468" s="8"/>
+      <c r="R468" s="10"/>
     </row>
     <row r="469">
-      <c r="R469" s="8"/>
+      <c r="R469" s="10"/>
     </row>
     <row r="470">
-      <c r="R470" s="8"/>
+      <c r="R470" s="10"/>
     </row>
     <row r="471">
-      <c r="R471" s="8"/>
+      <c r="R471" s="10"/>
     </row>
     <row r="472">
-      <c r="R472" s="8"/>
+      <c r="R472" s="10"/>
     </row>
     <row r="473">
-      <c r="R473" s="8"/>
+      <c r="R473" s="10"/>
     </row>
     <row r="474">
-      <c r="R474" s="8"/>
+      <c r="R474" s="10"/>
     </row>
     <row r="475">
-      <c r="R475" s="8"/>
+      <c r="R475" s="10"/>
     </row>
     <row r="476">
-      <c r="R476" s="8"/>
+      <c r="R476" s="10"/>
     </row>
     <row r="477">
-      <c r="R477" s="8"/>
+      <c r="R477" s="10"/>
     </row>
     <row r="478">
-      <c r="R478" s="8"/>
+      <c r="R478" s="10"/>
     </row>
     <row r="479">
-      <c r="R479" s="8"/>
+      <c r="R479" s="10"/>
     </row>
     <row r="480">
-      <c r="R480" s="8"/>
+      <c r="R480" s="10"/>
     </row>
     <row r="481">
-      <c r="R481" s="8"/>
+      <c r="R481" s="10"/>
     </row>
     <row r="482">
-      <c r="R482" s="8"/>
+      <c r="R482" s="10"/>
     </row>
     <row r="483">
-      <c r="R483" s="8"/>
+      <c r="R483" s="10"/>
     </row>
     <row r="484">
-      <c r="R484" s="8"/>
+      <c r="R484" s="10"/>
     </row>
     <row r="485">
-      <c r="R485" s="8"/>
+      <c r="R485" s="10"/>
     </row>
     <row r="486">
-      <c r="R486" s="8"/>
+      <c r="R486" s="10"/>
     </row>
     <row r="487">
-      <c r="R487" s="8"/>
+      <c r="R487" s="10"/>
     </row>
     <row r="488">
-      <c r="R488" s="8"/>
+      <c r="R488" s="10"/>
     </row>
     <row r="489">
-      <c r="R489" s="8"/>
+      <c r="R489" s="10"/>
     </row>
     <row r="490">
-      <c r="R490" s="8"/>
+      <c r="R490" s="10"/>
     </row>
     <row r="491">
-      <c r="R491" s="8"/>
+      <c r="R491" s="10"/>
     </row>
     <row r="492">
-      <c r="R492" s="8"/>
+      <c r="R492" s="10"/>
     </row>
     <row r="493">
-      <c r="R493" s="8"/>
+      <c r="R493" s="10"/>
     </row>
     <row r="494">
-      <c r="R494" s="8"/>
+      <c r="R494" s="10"/>
     </row>
     <row r="495">
-      <c r="R495" s="8"/>
+      <c r="R495" s="10"/>
     </row>
     <row r="496">
-      <c r="R496" s="8"/>
+      <c r="R496" s="10"/>
     </row>
     <row r="497">
-      <c r="R497" s="8"/>
+      <c r="R497" s="10"/>
     </row>
     <row r="498">
-      <c r="R498" s="8"/>
+      <c r="R498" s="10"/>
     </row>
     <row r="499">
-      <c r="R499" s="8"/>
+      <c r="R499" s="10"/>
     </row>
     <row r="500">
-      <c r="R500" s="8"/>
+      <c r="R500" s="10"/>
     </row>
     <row r="501">
-      <c r="R501" s="8"/>
+      <c r="R501" s="10"/>
     </row>
     <row r="502">
-      <c r="R502" s="8"/>
+      <c r="R502" s="10"/>
     </row>
     <row r="503">
-      <c r="R503" s="8"/>
+      <c r="R503" s="10"/>
     </row>
     <row r="504">
-      <c r="R504" s="8"/>
+      <c r="R504" s="10"/>
     </row>
     <row r="505">
-      <c r="R505" s="8"/>
+      <c r="R505" s="10"/>
     </row>
     <row r="506">
-      <c r="R506" s="8"/>
+      <c r="R506" s="10"/>
     </row>
     <row r="507">
-      <c r="R507" s="8"/>
+      <c r="R507" s="10"/>
     </row>
     <row r="508">
-      <c r="R508" s="8"/>
+      <c r="R508" s="10"/>
     </row>
     <row r="509">
-      <c r="R509" s="8"/>
+      <c r="R509" s="10"/>
     </row>
     <row r="510">
-      <c r="R510" s="8"/>
+      <c r="R510" s="10"/>
     </row>
     <row r="511">
-      <c r="R511" s="8"/>
+      <c r="R511" s="10"/>
     </row>
     <row r="512">
-      <c r="R512" s="8"/>
+      <c r="R512" s="10"/>
     </row>
     <row r="513">
-      <c r="R513" s="8"/>
+      <c r="R513" s="10"/>
     </row>
     <row r="514">
-      <c r="R514" s="8"/>
+      <c r="R514" s="10"/>
     </row>
     <row r="515">
-      <c r="R515" s="8"/>
+      <c r="R515" s="10"/>
     </row>
     <row r="516">
-      <c r="R516" s="8"/>
+      <c r="R516" s="10"/>
     </row>
     <row r="517">
-      <c r="R517" s="8"/>
+      <c r="R517" s="10"/>
     </row>
     <row r="518">
-      <c r="R518" s="8"/>
+      <c r="R518" s="10"/>
     </row>
     <row r="519">
-      <c r="R519" s="8"/>
+      <c r="R519" s="10"/>
     </row>
     <row r="520">
-      <c r="R520" s="8"/>
+      <c r="R520" s="10"/>
     </row>
     <row r="521">
-      <c r="R521" s="8"/>
+      <c r="R521" s="10"/>
     </row>
     <row r="522">
-      <c r="R522" s="8"/>
+      <c r="R522" s="10"/>
     </row>
     <row r="523">
-      <c r="R523" s="8"/>
+      <c r="R523" s="10"/>
     </row>
     <row r="524">
-      <c r="R524" s="8"/>
+      <c r="R524" s="10"/>
     </row>
     <row r="525">
-      <c r="R525" s="8"/>
+      <c r="R525" s="10"/>
     </row>
     <row r="526">
-      <c r="R526" s="8"/>
+      <c r="R526" s="10"/>
     </row>
     <row r="527">
-      <c r="R527" s="8"/>
+      <c r="R527" s="10"/>
     </row>
     <row r="528">
-      <c r="R528" s="8"/>
+      <c r="R528" s="10"/>
     </row>
     <row r="529">
-      <c r="R529" s="8"/>
+      <c r="R529" s="10"/>
     </row>
     <row r="530">
-      <c r="R530" s="8"/>
+      <c r="R530" s="10"/>
     </row>
     <row r="531">
-      <c r="R531" s="8"/>
+      <c r="R531" s="10"/>
     </row>
     <row r="532">
-      <c r="R532" s="8"/>
+      <c r="R532" s="10"/>
     </row>
     <row r="533">
-      <c r="R533" s="8"/>
+      <c r="R533" s="10"/>
     </row>
     <row r="534">
-      <c r="R534" s="8"/>
+      <c r="R534" s="10"/>
     </row>
     <row r="535">
-      <c r="R535" s="8"/>
+      <c r="R535" s="10"/>
     </row>
     <row r="536">
-      <c r="R536" s="8"/>
+      <c r="R536" s="10"/>
     </row>
     <row r="537">
-      <c r="R537" s="8"/>
+      <c r="R537" s="10"/>
     </row>
     <row r="538">
-      <c r="R538" s="8"/>
+      <c r="R538" s="10"/>
     </row>
     <row r="539">
-      <c r="R539" s="8"/>
+      <c r="R539" s="10"/>
     </row>
     <row r="540">
-      <c r="R540" s="8"/>
+      <c r="R540" s="10"/>
     </row>
     <row r="541">
-      <c r="R541" s="8"/>
+      <c r="R541" s="10"/>
     </row>
     <row r="542">
-      <c r="R542" s="8"/>
+      <c r="R542" s="10"/>
     </row>
     <row r="543">
-      <c r="R543" s="8"/>
+      <c r="R543" s="10"/>
     </row>
     <row r="544">
-      <c r="R544" s="8"/>
+      <c r="R544" s="10"/>
     </row>
     <row r="545">
-      <c r="R545" s="8"/>
+      <c r="R545" s="10"/>
     </row>
     <row r="546">
-      <c r="R546" s="8"/>
+      <c r="R546" s="10"/>
     </row>
     <row r="547">
-      <c r="R547" s="8"/>
+      <c r="R547" s="10"/>
     </row>
     <row r="548">
-      <c r="R548" s="8"/>
+      <c r="R548" s="10"/>
     </row>
     <row r="549">
-      <c r="R549" s="8"/>
+      <c r="R549" s="10"/>
     </row>
     <row r="550">
-      <c r="R550" s="8"/>
+      <c r="R550" s="10"/>
     </row>
     <row r="551">
-      <c r="R551" s="8"/>
+      <c r="R551" s="10"/>
     </row>
     <row r="552">
-      <c r="R552" s="8"/>
+      <c r="R552" s="10"/>
     </row>
     <row r="553">
-      <c r="R553" s="8"/>
+      <c r="R553" s="10"/>
     </row>
     <row r="554">
-      <c r="R554" s="8"/>
+      <c r="R554" s="10"/>
     </row>
     <row r="555">
-      <c r="R555" s="8"/>
+      <c r="R555" s="10"/>
     </row>
     <row r="556">
-      <c r="R556" s="8"/>
+      <c r="R556" s="10"/>
     </row>
     <row r="557">
-      <c r="R557" s="8"/>
+      <c r="R557" s="10"/>
     </row>
     <row r="558">
-      <c r="R558" s="8"/>
+      <c r="R558" s="10"/>
     </row>
     <row r="559">
-      <c r="R559" s="8"/>
+      <c r="R559" s="10"/>
     </row>
     <row r="560">
-      <c r="R560" s="8"/>
+      <c r="R560" s="10"/>
     </row>
     <row r="561">
-      <c r="R561" s="8"/>
+      <c r="R561" s="10"/>
     </row>
     <row r="562">
-      <c r="R562" s="8"/>
+      <c r="R562" s="10"/>
     </row>
     <row r="563">
-      <c r="R563" s="8"/>
+      <c r="R563" s="10"/>
     </row>
     <row r="564">
-      <c r="R564" s="8"/>
+      <c r="R564" s="10"/>
     </row>
     <row r="565">
-      <c r="R565" s="8"/>
+      <c r="R565" s="10"/>
     </row>
     <row r="566">
-      <c r="R566" s="8"/>
+      <c r="R566" s="10"/>
     </row>
     <row r="567">
-      <c r="R567" s="8"/>
+      <c r="R567" s="10"/>
     </row>
     <row r="568">
-      <c r="R568" s="8"/>
+      <c r="R568" s="10"/>
     </row>
     <row r="569">
-      <c r="R569" s="8"/>
+      <c r="R569" s="10"/>
     </row>
     <row r="570">
-      <c r="R570" s="8"/>
+      <c r="R570" s="10"/>
     </row>
     <row r="571">
-      <c r="R571" s="8"/>
+      <c r="R571" s="10"/>
     </row>
     <row r="572">
-      <c r="R572" s="8"/>
+      <c r="R572" s="10"/>
     </row>
     <row r="573">
-      <c r="R573" s="8"/>
+      <c r="R573" s="10"/>
     </row>
     <row r="574">
-      <c r="R574" s="8"/>
+      <c r="R574" s="10"/>
     </row>
     <row r="575">
-      <c r="R575" s="8"/>
+      <c r="R575" s="10"/>
     </row>
     <row r="576">
-      <c r="R576" s="8"/>
+      <c r="R576" s="10"/>
     </row>
     <row r="577">
-      <c r="R577" s="8"/>
+      <c r="R577" s="10"/>
     </row>
     <row r="578">
-      <c r="R578" s="8"/>
+      <c r="R578" s="10"/>
     </row>
     <row r="579">
-      <c r="R579" s="8"/>
+      <c r="R579" s="10"/>
     </row>
     <row r="580">
-      <c r="R580" s="8"/>
+      <c r="R580" s="10"/>
     </row>
     <row r="581">
-      <c r="R581" s="8"/>
+      <c r="R581" s="10"/>
     </row>
     <row r="582">
-      <c r="R582" s="8"/>
+      <c r="R582" s="10"/>
     </row>
     <row r="583">
-      <c r="R583" s="8"/>
+      <c r="R583" s="10"/>
     </row>
     <row r="584">
-      <c r="R584" s="8"/>
+      <c r="R584" s="10"/>
     </row>
     <row r="585">
-      <c r="R585" s="8"/>
+      <c r="R585" s="10"/>
     </row>
     <row r="586">
-      <c r="R586" s="8"/>
+      <c r="R586" s="10"/>
     </row>
     <row r="587">
-      <c r="R587" s="8"/>
+      <c r="R587" s="10"/>
     </row>
     <row r="588">
-      <c r="R588" s="8"/>
+      <c r="R588" s="10"/>
     </row>
     <row r="589">
-      <c r="R589" s="8"/>
+      <c r="R589" s="10"/>
     </row>
     <row r="590">
-      <c r="R590" s="8"/>
+      <c r="R590" s="10"/>
     </row>
     <row r="591">
-      <c r="R591" s="8"/>
+      <c r="R591" s="10"/>
     </row>
     <row r="592">
-      <c r="R592" s="8"/>
+      <c r="R592" s="10"/>
     </row>
     <row r="593">
-      <c r="R593" s="8"/>
+      <c r="R593" s="10"/>
     </row>
     <row r="594">
-      <c r="R594" s="8"/>
+      <c r="R594" s="10"/>
     </row>
     <row r="595">
-      <c r="R595" s="8"/>
+      <c r="R595" s="10"/>
     </row>
     <row r="596">
-      <c r="R596" s="8"/>
+      <c r="R596" s="10"/>
     </row>
     <row r="597">
-      <c r="R597" s="8"/>
+      <c r="R597" s="10"/>
     </row>
     <row r="598">
-      <c r="R598" s="8"/>
+      <c r="R598" s="10"/>
     </row>
     <row r="599">
-      <c r="R599" s="8"/>
+      <c r="R599" s="10"/>
     </row>
     <row r="600">
-      <c r="R600" s="8"/>
+      <c r="R600" s="10"/>
     </row>
     <row r="601">
-      <c r="R601" s="8"/>
+      <c r="R601" s="10"/>
     </row>
     <row r="602">
-      <c r="R602" s="8"/>
+      <c r="R602" s="10"/>
     </row>
     <row r="603">
-      <c r="R603" s="8"/>
+      <c r="R603" s="10"/>
     </row>
     <row r="604">
-      <c r="R604" s="8"/>
+      <c r="R604" s="10"/>
     </row>
     <row r="605">
-      <c r="R605" s="8"/>
+      <c r="R605" s="10"/>
     </row>
     <row r="606">
-      <c r="R606" s="8"/>
+      <c r="R606" s="10"/>
     </row>
     <row r="607">
-      <c r="R607" s="8"/>
+      <c r="R607" s="10"/>
     </row>
     <row r="608">
-      <c r="R608" s="8"/>
+      <c r="R608" s="10"/>
     </row>
     <row r="609">
-      <c r="R609" s="8"/>
+      <c r="R609" s="10"/>
     </row>
     <row r="610">
-      <c r="R610" s="8"/>
+      <c r="R610" s="10"/>
     </row>
     <row r="611">
-      <c r="R611" s="8"/>
+      <c r="R611" s="10"/>
     </row>
     <row r="612">
-      <c r="R612" s="8"/>
+      <c r="R612" s="10"/>
     </row>
     <row r="613">
-      <c r="R613" s="8"/>
+      <c r="R613" s="10"/>
     </row>
     <row r="614">
-      <c r="R614" s="8"/>
+      <c r="R614" s="10"/>
     </row>
     <row r="615">
-      <c r="R615" s="8"/>
+      <c r="R615" s="10"/>
     </row>
     <row r="616">
-      <c r="R616" s="8"/>
+      <c r="R616" s="10"/>
     </row>
     <row r="617">
-      <c r="R617" s="8"/>
+      <c r="R617" s="10"/>
     </row>
     <row r="618">
-      <c r="R618" s="8"/>
+      <c r="R618" s="10"/>
     </row>
     <row r="619">
-      <c r="R619" s="8"/>
+      <c r="R619" s="10"/>
     </row>
     <row r="620">
-      <c r="R620" s="8"/>
+      <c r="R620" s="10"/>
     </row>
     <row r="621">
-      <c r="R621" s="8"/>
+      <c r="R621" s="10"/>
     </row>
     <row r="622">
-      <c r="R622" s="8"/>
+      <c r="R622" s="10"/>
     </row>
     <row r="623">
-      <c r="R623" s="8"/>
+      <c r="R623" s="10"/>
     </row>
     <row r="624">
-      <c r="R624" s="8"/>
+      <c r="R624" s="10"/>
     </row>
     <row r="625">
-      <c r="R625" s="8"/>
+      <c r="R625" s="10"/>
     </row>
     <row r="626">
-      <c r="R626" s="8"/>
+      <c r="R626" s="10"/>
     </row>
     <row r="627">
-      <c r="R627" s="8"/>
+      <c r="R627" s="10"/>
     </row>
     <row r="628">
-      <c r="R628" s="8"/>
+      <c r="R628" s="10"/>
     </row>
     <row r="629">
-      <c r="R629" s="8"/>
+      <c r="R629" s="10"/>
     </row>
     <row r="630">
-      <c r="R630" s="8"/>
+      <c r="R630" s="10"/>
     </row>
     <row r="631">
-      <c r="R631" s="8"/>
+      <c r="R631" s="10"/>
     </row>
     <row r="632">
-      <c r="R632" s="8"/>
+      <c r="R632" s="10"/>
     </row>
     <row r="633">
-      <c r="R633" s="8"/>
+      <c r="R633" s="10"/>
     </row>
     <row r="634">
-      <c r="R634" s="8"/>
+      <c r="R634" s="10"/>
     </row>
     <row r="635">
-      <c r="R635" s="8"/>
+      <c r="R635" s="10"/>
     </row>
     <row r="636">
-      <c r="R636" s="8"/>
+      <c r="R636" s="10"/>
     </row>
     <row r="637">
-      <c r="R637" s="8"/>
+      <c r="R637" s="10"/>
     </row>
     <row r="638">
-      <c r="R638" s="8"/>
+      <c r="R638" s="10"/>
     </row>
     <row r="639">
-      <c r="R639" s="8"/>
+      <c r="R639" s="10"/>
     </row>
     <row r="640">
-      <c r="R640" s="8"/>
+      <c r="R640" s="10"/>
     </row>
     <row r="641">
-      <c r="R641" s="8"/>
+      <c r="R641" s="10"/>
     </row>
     <row r="642">
-      <c r="R642" s="8"/>
+      <c r="R642" s="10"/>
     </row>
     <row r="643">
-      <c r="R643" s="8"/>
+      <c r="R643" s="10"/>
     </row>
     <row r="644">
-      <c r="R644" s="8"/>
+      <c r="R644" s="10"/>
     </row>
     <row r="645">
-      <c r="R645" s="8"/>
+      <c r="R645" s="10"/>
     </row>
     <row r="646">
-      <c r="R646" s="8"/>
+      <c r="R646" s="10"/>
     </row>
     <row r="647">
-      <c r="R647" s="8"/>
+      <c r="R647" s="10"/>
     </row>
     <row r="648">
-      <c r="R648" s="8"/>
+      <c r="R648" s="10"/>
     </row>
     <row r="649">
-      <c r="R649" s="8"/>
+      <c r="R649" s="10"/>
     </row>
     <row r="650">
-      <c r="R650" s="8"/>
+      <c r="R650" s="10"/>
     </row>
     <row r="651">
-      <c r="R651" s="8"/>
+      <c r="R651" s="10"/>
     </row>
     <row r="652">
-      <c r="R652" s="8"/>
+      <c r="R652" s="10"/>
     </row>
     <row r="653">
-      <c r="R653" s="8"/>
+      <c r="R653" s="10"/>
     </row>
     <row r="654">
-      <c r="R654" s="8"/>
+      <c r="R654" s="10"/>
     </row>
     <row r="655">
-      <c r="R655" s="8"/>
+      <c r="R655" s="10"/>
     </row>
     <row r="656">
-      <c r="R656" s="8"/>
+      <c r="R656" s="10"/>
     </row>
     <row r="657">
-      <c r="R657" s="8"/>
+      <c r="R657" s="10"/>
     </row>
     <row r="658">
-      <c r="R658" s="8"/>
+      <c r="R658" s="10"/>
     </row>
     <row r="659">
-      <c r="R659" s="8"/>
+      <c r="R659" s="10"/>
     </row>
     <row r="660">
-      <c r="R660" s="8"/>
+      <c r="R660" s="10"/>
     </row>
     <row r="661">
-      <c r="R661" s="8"/>
+      <c r="R661" s="10"/>
     </row>
     <row r="662">
-      <c r="R662" s="8"/>
+      <c r="R662" s="10"/>
     </row>
     <row r="663">
-      <c r="R663" s="8"/>
+      <c r="R663" s="10"/>
     </row>
     <row r="664">
-      <c r="R664" s="8"/>
+      <c r="R664" s="10"/>
     </row>
     <row r="665">
-      <c r="R665" s="8"/>
+      <c r="R665" s="10"/>
     </row>
     <row r="666">
-      <c r="R666" s="8"/>
+      <c r="R666" s="10"/>
     </row>
     <row r="667">
-      <c r="R667" s="8"/>
+      <c r="R667" s="10"/>
     </row>
     <row r="668">
-      <c r="R668" s="8"/>
+      <c r="R668" s="10"/>
     </row>
     <row r="669">
-      <c r="R669" s="8"/>
+      <c r="R669" s="10"/>
     </row>
     <row r="670">
-      <c r="R670" s="8"/>
+      <c r="R670" s="10"/>
     </row>
     <row r="671">
-      <c r="R671" s="8"/>
+      <c r="R671" s="10"/>
     </row>
     <row r="672">
-      <c r="R672" s="8"/>
+      <c r="R672" s="10"/>
     </row>
     <row r="673">
-      <c r="R673" s="8"/>
+      <c r="R673" s="10"/>
     </row>
     <row r="674">
-      <c r="R674" s="8"/>
+      <c r="R674" s="10"/>
     </row>
     <row r="675">
-      <c r="R675" s="8"/>
+      <c r="R675" s="10"/>
     </row>
     <row r="676">
-      <c r="R676" s="8"/>
+      <c r="R676" s="10"/>
     </row>
     <row r="677">
-      <c r="R677" s="8"/>
+      <c r="R677" s="10"/>
     </row>
     <row r="678">
-      <c r="R678" s="8"/>
+      <c r="R678" s="10"/>
     </row>
     <row r="679">
-      <c r="R679" s="8"/>
+      <c r="R679" s="10"/>
     </row>
     <row r="680">
-      <c r="R680" s="8"/>
+      <c r="R680" s="10"/>
     </row>
     <row r="681">
-      <c r="R681" s="8"/>
+      <c r="R681" s="10"/>
     </row>
     <row r="682">
-      <c r="R682" s="8"/>
+      <c r="R682" s="10"/>
     </row>
     <row r="683">
-      <c r="R683" s="8"/>
+      <c r="R683" s="10"/>
     </row>
     <row r="684">
-      <c r="R684" s="8"/>
+      <c r="R684" s="10"/>
     </row>
     <row r="685">
-      <c r="R685" s="8"/>
+      <c r="R685" s="10"/>
     </row>
     <row r="686">
-      <c r="R686" s="8"/>
+      <c r="R686" s="10"/>
     </row>
     <row r="687">
-      <c r="R687" s="8"/>
+      <c r="R687" s="10"/>
     </row>
     <row r="688">
-      <c r="R688" s="8"/>
+      <c r="R688" s="10"/>
     </row>
     <row r="689">
-      <c r="R689" s="8"/>
+      <c r="R689" s="10"/>
     </row>
     <row r="690">
-      <c r="R690" s="8"/>
+      <c r="R690" s="10"/>
     </row>
     <row r="691">
-      <c r="R691" s="8"/>
+      <c r="R691" s="10"/>
     </row>
     <row r="692">
-      <c r="R692" s="8"/>
+      <c r="R692" s="10"/>
     </row>
     <row r="693">
-      <c r="R693" s="8"/>
+      <c r="R693" s="10"/>
     </row>
     <row r="694">
-      <c r="R694" s="8"/>
+      <c r="R694" s="10"/>
     </row>
     <row r="695">
-      <c r="R695" s="8"/>
+      <c r="R695" s="10"/>
     </row>
     <row r="696">
-      <c r="R696" s="8"/>
+      <c r="R696" s="10"/>
     </row>
     <row r="697">
-      <c r="R697" s="8"/>
+      <c r="R697" s="10"/>
     </row>
     <row r="698">
-      <c r="R698" s="8"/>
+      <c r="R698" s="10"/>
     </row>
     <row r="699">
-      <c r="R699" s="8"/>
+      <c r="R699" s="10"/>
     </row>
     <row r="700">
-      <c r="R700" s="8"/>
+      <c r="R700" s="10"/>
     </row>
     <row r="701">
-      <c r="R701" s="8"/>
+      <c r="R701" s="10"/>
     </row>
     <row r="702">
-      <c r="R702" s="8"/>
+      <c r="R702" s="10"/>
     </row>
     <row r="703">
-      <c r="R703" s="8"/>
+      <c r="R703" s="10"/>
     </row>
     <row r="704">
-      <c r="R704" s="8"/>
+      <c r="R704" s="10"/>
     </row>
     <row r="705">
-      <c r="R705" s="8"/>
+      <c r="R705" s="10"/>
     </row>
     <row r="706">
-      <c r="R706" s="8"/>
+      <c r="R706" s="10"/>
     </row>
     <row r="707">
-      <c r="R707" s="8"/>
+      <c r="R707" s="10"/>
     </row>
     <row r="708">
-      <c r="R708" s="8"/>
+      <c r="R708" s="10"/>
     </row>
     <row r="709">
-      <c r="R709" s="8"/>
+      <c r="R709" s="10"/>
     </row>
     <row r="710">
-      <c r="R710" s="8"/>
+      <c r="R710" s="10"/>
     </row>
     <row r="711">
-      <c r="R711" s="8"/>
+      <c r="R711" s="10"/>
     </row>
     <row r="712">
-      <c r="R712" s="8"/>
+      <c r="R712" s="10"/>
     </row>
     <row r="713">
-      <c r="R713" s="8"/>
+      <c r="R713" s="10"/>
     </row>
     <row r="714">
-      <c r="R714" s="8"/>
+      <c r="R714" s="10"/>
     </row>
     <row r="715">
-      <c r="R715" s="8"/>
+      <c r="R715" s="10"/>
     </row>
     <row r="716">
-      <c r="R716" s="8"/>
+      <c r="R716" s="10"/>
     </row>
     <row r="717">
-      <c r="R717" s="8"/>
+      <c r="R717" s="10"/>
     </row>
     <row r="718">
-      <c r="R718" s="8"/>
+      <c r="R718" s="10"/>
     </row>
     <row r="719">
-      <c r="R719" s="8"/>
+      <c r="R719" s="10"/>
     </row>
     <row r="720">
-      <c r="R720" s="8"/>
+      <c r="R720" s="10"/>
     </row>
     <row r="721">
-      <c r="R721" s="8"/>
+      <c r="R721" s="10"/>
     </row>
     <row r="722">
-      <c r="R722" s="8"/>
+      <c r="R722" s="10"/>
     </row>
     <row r="723">
-      <c r="R723" s="8"/>
+      <c r="R723" s="10"/>
     </row>
     <row r="724">
-      <c r="R724" s="8"/>
+      <c r="R724" s="10"/>
     </row>
     <row r="725">
-      <c r="R725" s="8"/>
+      <c r="R725" s="10"/>
     </row>
     <row r="726">
-      <c r="R726" s="8"/>
+      <c r="R726" s="10"/>
     </row>
     <row r="727">
-      <c r="R727" s="8"/>
+      <c r="R727" s="10"/>
     </row>
     <row r="728">
-      <c r="R728" s="8"/>
+      <c r="R728" s="10"/>
     </row>
     <row r="729">
-      <c r="R729" s="8"/>
+      <c r="R729" s="10"/>
     </row>
     <row r="730">
-      <c r="R730" s="8"/>
+      <c r="R730" s="10"/>
     </row>
     <row r="731">
-      <c r="R731" s="8"/>
+      <c r="R731" s="10"/>
     </row>
     <row r="732">
-      <c r="R732" s="8"/>
+      <c r="R732" s="10"/>
     </row>
     <row r="733">
-      <c r="R733" s="8"/>
+      <c r="R733" s="10"/>
     </row>
     <row r="734">
-      <c r="R734" s="8"/>
+      <c r="R734" s="10"/>
     </row>
     <row r="735">
-      <c r="R735" s="8"/>
+      <c r="R735" s="10"/>
     </row>
     <row r="736">
-      <c r="R736" s="8"/>
+      <c r="R736" s="10"/>
     </row>
     <row r="737">
-      <c r="R737" s="8"/>
+      <c r="R737" s="10"/>
     </row>
     <row r="738">
-      <c r="R738" s="8"/>
+      <c r="R738" s="10"/>
     </row>
     <row r="739">
-      <c r="R739" s="8"/>
+      <c r="R739" s="10"/>
     </row>
     <row r="740">
-      <c r="R740" s="8"/>
+      <c r="R740" s="10"/>
     </row>
     <row r="741">
-      <c r="R741" s="8"/>
+      <c r="R741" s="10"/>
     </row>
     <row r="742">
-      <c r="R742" s="8"/>
+      <c r="R742" s="10"/>
     </row>
     <row r="743">
-      <c r="R743" s="8"/>
+      <c r="R743" s="10"/>
     </row>
     <row r="744">
-      <c r="R744" s="8"/>
+      <c r="R744" s="10"/>
     </row>
     <row r="745">
-      <c r="R745" s="8"/>
+      <c r="R745" s="10"/>
     </row>
     <row r="746">
-      <c r="R746" s="8"/>
+      <c r="R746" s="10"/>
     </row>
     <row r="747">
-      <c r="R747" s="8"/>
+      <c r="R747" s="10"/>
     </row>
     <row r="748">
-      <c r="R748" s="8"/>
+      <c r="R748" s="10"/>
     </row>
     <row r="749">
-      <c r="R749" s="8"/>
+      <c r="R749" s="10"/>
     </row>
     <row r="750">
-      <c r="R750" s="8"/>
+      <c r="R750" s="10"/>
     </row>
     <row r="751">
-      <c r="R751" s="8"/>
+      <c r="R751" s="10"/>
     </row>
     <row r="752">
-      <c r="R752" s="8"/>
+      <c r="R752" s="10"/>
     </row>
     <row r="753">
-      <c r="R753" s="8"/>
+      <c r="R753" s="10"/>
     </row>
     <row r="754">
-      <c r="R754" s="8"/>
+      <c r="R754" s="10"/>
     </row>
     <row r="755">
-      <c r="R755" s="8"/>
+      <c r="R755" s="10"/>
     </row>
     <row r="756">
-      <c r="R756" s="8"/>
+      <c r="R756" s="10"/>
     </row>
     <row r="757">
-      <c r="R757" s="8"/>
+      <c r="R757" s="10"/>
     </row>
     <row r="758">
-      <c r="R758" s="8"/>
+      <c r="R758" s="10"/>
     </row>
     <row r="759">
-      <c r="R759" s="8"/>
+      <c r="R759" s="10"/>
     </row>
     <row r="760">
-      <c r="R760" s="8"/>
+      <c r="R760" s="10"/>
     </row>
     <row r="761">
-      <c r="R761" s="8"/>
+      <c r="R761" s="10"/>
     </row>
     <row r="762">
-      <c r="R762" s="8"/>
+      <c r="R762" s="10"/>
     </row>
     <row r="763">
-      <c r="R763" s="8"/>
+      <c r="R763" s="10"/>
     </row>
     <row r="764">
-      <c r="R764" s="8"/>
+      <c r="R764" s="10"/>
     </row>
     <row r="765">
-      <c r="R765" s="8"/>
+      <c r="R765" s="10"/>
     </row>
     <row r="766">
-      <c r="R766" s="8"/>
+      <c r="R766" s="10"/>
     </row>
     <row r="767">
-      <c r="R767" s="8"/>
+      <c r="R767" s="10"/>
     </row>
     <row r="768">
-      <c r="R768" s="8"/>
+      <c r="R768" s="10"/>
     </row>
     <row r="769">
-      <c r="R769" s="8"/>
+      <c r="R769" s="10"/>
     </row>
     <row r="770">
-      <c r="R770" s="8"/>
+      <c r="R770" s="10"/>
     </row>
     <row r="771">
-      <c r="R771" s="8"/>
+      <c r="R771" s="10"/>
     </row>
     <row r="772">
-      <c r="R772" s="8"/>
+      <c r="R772" s="10"/>
     </row>
     <row r="773">
-      <c r="R773" s="8"/>
+      <c r="R773" s="10"/>
     </row>
     <row r="774">
-      <c r="R774" s="8"/>
+      <c r="R774" s="10"/>
     </row>
     <row r="775">
-      <c r="R775" s="8"/>
+      <c r="R775" s="10"/>
     </row>
     <row r="776">
-      <c r="R776" s="8"/>
+      <c r="R776" s="10"/>
     </row>
     <row r="777">
-      <c r="R777" s="8"/>
+      <c r="R777" s="10"/>
     </row>
     <row r="778">
-      <c r="R778" s="8"/>
+      <c r="R778" s="10"/>
     </row>
     <row r="779">
-      <c r="R779" s="8"/>
+      <c r="R779" s="10"/>
     </row>
     <row r="780">
-      <c r="R780" s="8"/>
+      <c r="R780" s="10"/>
     </row>
     <row r="781">
-      <c r="R781" s="8"/>
+      <c r="R781" s="10"/>
     </row>
     <row r="782">
-      <c r="R782" s="8"/>
+      <c r="R782" s="10"/>
     </row>
     <row r="783">
-      <c r="R783" s="8"/>
+      <c r="R783" s="10"/>
     </row>
     <row r="784">
-      <c r="R784" s="8"/>
+      <c r="R784" s="10"/>
     </row>
     <row r="785">
-      <c r="R785" s="8"/>
+      <c r="R785" s="10"/>
     </row>
     <row r="786">
-      <c r="R786" s="8"/>
+      <c r="R786" s="10"/>
     </row>
     <row r="787">
-      <c r="R787" s="8"/>
+      <c r="R787" s="10"/>
     </row>
     <row r="788">
-      <c r="R788" s="8"/>
+      <c r="R788" s="10"/>
     </row>
     <row r="789">
-      <c r="R789" s="8"/>
+      <c r="R789" s="10"/>
     </row>
     <row r="790">
-      <c r="R790" s="8"/>
+      <c r="R790" s="10"/>
     </row>
     <row r="791">
-      <c r="R791" s="8"/>
+      <c r="R791" s="10"/>
     </row>
     <row r="792">
-      <c r="R792" s="8"/>
+      <c r="R792" s="10"/>
     </row>
     <row r="793">
-      <c r="R793" s="8"/>
+      <c r="R793" s="10"/>
     </row>
     <row r="794">
-      <c r="R794" s="8"/>
+      <c r="R794" s="10"/>
     </row>
     <row r="795">
-      <c r="R795" s="8"/>
+      <c r="R795" s="10"/>
     </row>
     <row r="796">
-      <c r="R796" s="8"/>
+      <c r="R796" s="10"/>
     </row>
     <row r="797">
-      <c r="R797" s="8"/>
+      <c r="R797" s="10"/>
     </row>
     <row r="798">
-      <c r="R798" s="8"/>
+      <c r="R798" s="10"/>
     </row>
     <row r="799">
-      <c r="R799" s="8"/>
+      <c r="R799" s="10"/>
     </row>
     <row r="800">
-      <c r="R800" s="8"/>
+      <c r="R800" s="10"/>
     </row>
     <row r="801">
-      <c r="R801" s="8"/>
+      <c r="R801" s="10"/>
     </row>
     <row r="802">
-      <c r="R802" s="8"/>
+      <c r="R802" s="10"/>
     </row>
     <row r="803">
-      <c r="R803" s="8"/>
+      <c r="R803" s="10"/>
     </row>
     <row r="804">
-      <c r="R804" s="8"/>
+      <c r="R804" s="10"/>
     </row>
     <row r="805">
-      <c r="R805" s="8"/>
+      <c r="R805" s="10"/>
     </row>
     <row r="806">
-      <c r="R806" s="8"/>
+      <c r="R806" s="10"/>
     </row>
     <row r="807">
-      <c r="R807" s="8"/>
+      <c r="R807" s="10"/>
     </row>
     <row r="808">
-      <c r="R808" s="8"/>
+      <c r="R808" s="10"/>
     </row>
     <row r="809">
-      <c r="R809" s="8"/>
+      <c r="R809" s="10"/>
     </row>
     <row r="810">
-      <c r="R810" s="8"/>
+      <c r="R810" s="10"/>
     </row>
     <row r="811">
-      <c r="R811" s="8"/>
+      <c r="R811" s="10"/>
     </row>
     <row r="812">
-      <c r="R812" s="8"/>
+      <c r="R812" s="10"/>
     </row>
     <row r="813">
-      <c r="R813" s="8"/>
+      <c r="R813" s="10"/>
     </row>
     <row r="814">
-      <c r="R814" s="8"/>
+      <c r="R814" s="10"/>
     </row>
     <row r="815">
-      <c r="R815" s="8"/>
+      <c r="R815" s="10"/>
     </row>
     <row r="816">
-      <c r="R816" s="8"/>
+      <c r="R816" s="10"/>
     </row>
     <row r="817">
-      <c r="R817" s="8"/>
+      <c r="R817" s="10"/>
     </row>
     <row r="818">
-      <c r="R818" s="8"/>
+      <c r="R818" s="10"/>
     </row>
     <row r="819">
-      <c r="R819" s="8"/>
+      <c r="R819" s="10"/>
     </row>
     <row r="820">
-      <c r="R820" s="8"/>
+      <c r="R820" s="10"/>
     </row>
     <row r="821">
-      <c r="R821" s="8"/>
+      <c r="R821" s="10"/>
     </row>
     <row r="822">
-      <c r="R822" s="8"/>
+      <c r="R822" s="10"/>
     </row>
     <row r="823">
-      <c r="R823" s="8"/>
+      <c r="R823" s="10"/>
     </row>
     <row r="824">
-      <c r="R824" s="8"/>
+      <c r="R824" s="10"/>
     </row>
     <row r="825">
-      <c r="R825" s="8"/>
+      <c r="R825" s="10"/>
     </row>
     <row r="826">
-      <c r="R826" s="8"/>
+      <c r="R826" s="10"/>
     </row>
     <row r="827">
-      <c r="R827" s="8"/>
+      <c r="R827" s="10"/>
     </row>
     <row r="828">
-      <c r="R828" s="8"/>
+      <c r="R828" s="10"/>
     </row>
     <row r="829">
-      <c r="R829" s="8"/>
+      <c r="R829" s="10"/>
     </row>
     <row r="830">
-      <c r="R830" s="8"/>
+      <c r="R830" s="10"/>
     </row>
     <row r="831">
-      <c r="R831" s="8"/>
+      <c r="R831" s="10"/>
     </row>
     <row r="832">
-      <c r="R832" s="8"/>
+      <c r="R832" s="10"/>
     </row>
     <row r="833">
-      <c r="R833" s="8"/>
+      <c r="R833" s="10"/>
     </row>
     <row r="834">
-      <c r="R834" s="8"/>
+      <c r="R834" s="10"/>
     </row>
     <row r="835">
-      <c r="R835" s="8"/>
+      <c r="R835" s="10"/>
     </row>
     <row r="836">
-      <c r="R836" s="8"/>
+      <c r="R836" s="10"/>
     </row>
     <row r="837">
-      <c r="R837" s="8"/>
+      <c r="R837" s="10"/>
     </row>
     <row r="838">
-      <c r="R838" s="8"/>
+      <c r="R838" s="10"/>
     </row>
     <row r="839">
-      <c r="R839" s="8"/>
+      <c r="R839" s="10"/>
     </row>
     <row r="840">
-      <c r="R840" s="8"/>
+      <c r="R840" s="10"/>
     </row>
     <row r="841">
-      <c r="R841" s="8"/>
+      <c r="R841" s="10"/>
     </row>
     <row r="842">
-      <c r="R842" s="8"/>
+      <c r="R842" s="10"/>
     </row>
     <row r="843">
-      <c r="R843" s="8"/>
+      <c r="R843" s="10"/>
     </row>
     <row r="844">
-      <c r="R844" s="8"/>
+      <c r="R844" s="10"/>
     </row>
     <row r="845">
-      <c r="R845" s="8"/>
+      <c r="R845" s="10"/>
     </row>
     <row r="846">
-      <c r="R846" s="8"/>
+      <c r="R846" s="10"/>
     </row>
     <row r="847">
-      <c r="R847" s="8"/>
+      <c r="R847" s="10"/>
     </row>
     <row r="848">
-      <c r="R848" s="8"/>
+      <c r="R848" s="10"/>
     </row>
     <row r="849">
-      <c r="R849" s="8"/>
+      <c r="R849" s="10"/>
     </row>
     <row r="850">
-      <c r="R850" s="8"/>
+      <c r="R850" s="10"/>
     </row>
     <row r="851">
-      <c r="R851" s="8"/>
+      <c r="R851" s="10"/>
     </row>
     <row r="852">
-      <c r="R852" s="8"/>
+      <c r="R852" s="10"/>
     </row>
     <row r="853">
-      <c r="R853" s="8"/>
+      <c r="R853" s="10"/>
     </row>
     <row r="854">
-      <c r="R854" s="8"/>
+      <c r="R854" s="10"/>
     </row>
     <row r="855">
-      <c r="R855" s="8"/>
+      <c r="R855" s="10"/>
     </row>
     <row r="856">
-      <c r="R856" s="8"/>
+      <c r="R856" s="10"/>
     </row>
     <row r="857">
-      <c r="R857" s="8"/>
+      <c r="R857" s="10"/>
     </row>
     <row r="858">
-      <c r="R858" s="8"/>
+      <c r="R858" s="10"/>
     </row>
     <row r="859">
-      <c r="R859" s="8"/>
+      <c r="R859" s="10"/>
     </row>
     <row r="860">
-      <c r="R860" s="8"/>
+      <c r="R860" s="10"/>
     </row>
     <row r="861">
-      <c r="R861" s="8"/>
+      <c r="R861" s="10"/>
     </row>
     <row r="862">
-      <c r="R862" s="8"/>
+      <c r="R862" s="10"/>
     </row>
     <row r="863">
-      <c r="R863" s="8"/>
+      <c r="R863" s="10"/>
     </row>
     <row r="864">
-      <c r="R864" s="8"/>
+      <c r="R864" s="10"/>
     </row>
     <row r="865">
-      <c r="R865" s="8"/>
+      <c r="R865" s="10"/>
     </row>
     <row r="866">
-      <c r="R866" s="8"/>
+      <c r="R866" s="10"/>
     </row>
     <row r="867">
-      <c r="R867" s="8"/>
+      <c r="R867" s="10"/>
     </row>
     <row r="868">
-      <c r="R868" s="8"/>
+      <c r="R868" s="10"/>
     </row>
     <row r="869">
-      <c r="R869" s="8"/>
+      <c r="R869" s="10"/>
     </row>
     <row r="870">
-      <c r="R870" s="8"/>
+      <c r="R870" s="10"/>
     </row>
     <row r="871">
-      <c r="R871" s="8"/>
+      <c r="R871" s="10"/>
     </row>
     <row r="872">
-      <c r="R872" s="8"/>
+      <c r="R872" s="10"/>
     </row>
     <row r="873">
-      <c r="R873" s="8"/>
+      <c r="R873" s="10"/>
     </row>
     <row r="874">
-      <c r="R874" s="8"/>
+      <c r="R874" s="10"/>
     </row>
     <row r="875">
-      <c r="R875" s="8"/>
+      <c r="R875" s="10"/>
     </row>
     <row r="876">
-      <c r="R876" s="8"/>
+      <c r="R876" s="10"/>
     </row>
     <row r="877">
-      <c r="R877" s="8"/>
+      <c r="R877" s="10"/>
     </row>
     <row r="878">
-      <c r="R878" s="8"/>
+      <c r="R878" s="10"/>
     </row>
     <row r="879">
-      <c r="R879" s="8"/>
+      <c r="R879" s="10"/>
     </row>
     <row r="880">
-      <c r="R880" s="8"/>
+      <c r="R880" s="10"/>
     </row>
     <row r="881">
-      <c r="R881" s="8"/>
+      <c r="R881" s="10"/>
     </row>
     <row r="882">
-      <c r="R882" s="8"/>
+      <c r="R882" s="10"/>
     </row>
     <row r="883">
-      <c r="R883" s="8"/>
+      <c r="R883" s="10"/>
     </row>
     <row r="884">
-      <c r="R884" s="8"/>
+      <c r="R884" s="10"/>
     </row>
     <row r="885">
-      <c r="R885" s="8"/>
+      <c r="R885" s="10"/>
     </row>
     <row r="886">
-      <c r="R886" s="8"/>
+      <c r="R886" s="10"/>
     </row>
     <row r="887">
-      <c r="R887" s="8"/>
+      <c r="R887" s="10"/>
     </row>
     <row r="888">
-      <c r="R888" s="8"/>
+      <c r="R888" s="10"/>
     </row>
     <row r="889">
-      <c r="R889" s="8"/>
+      <c r="R889" s="10"/>
     </row>
     <row r="890">
-      <c r="R890" s="8"/>
+      <c r="R890" s="10"/>
     </row>
     <row r="891">
-      <c r="R891" s="8"/>
+      <c r="R891" s="10"/>
     </row>
     <row r="892">
-      <c r="R892" s="8"/>
+      <c r="R892" s="10"/>
     </row>
     <row r="893">
-      <c r="R893" s="8"/>
+      <c r="R893" s="10"/>
     </row>
     <row r="894">
-      <c r="R894" s="8"/>
+      <c r="R894" s="10"/>
     </row>
     <row r="895">
-      <c r="R895" s="8"/>
+      <c r="R895" s="10"/>
     </row>
     <row r="896">
-      <c r="R896" s="8"/>
+      <c r="R896" s="10"/>
     </row>
     <row r="897">
-      <c r="R897" s="8"/>
+      <c r="R897" s="10"/>
     </row>
     <row r="898">
-      <c r="R898" s="8"/>
+      <c r="R898" s="10"/>
     </row>
     <row r="899">
-      <c r="R899" s="8"/>
+      <c r="R899" s="10"/>
     </row>
     <row r="900">
-      <c r="R900" s="8"/>
+      <c r="R900" s="10"/>
     </row>
     <row r="901">
-      <c r="R901" s="8"/>
+      <c r="R901" s="10"/>
     </row>
     <row r="902">
-      <c r="R902" s="8"/>
+      <c r="R902" s="10"/>
     </row>
     <row r="903">
-      <c r="R903" s="8"/>
+      <c r="R903" s="10"/>
     </row>
     <row r="904">
-      <c r="R904" s="8"/>
+      <c r="R904" s="10"/>
     </row>
     <row r="905">
-      <c r="R905" s="8"/>
+      <c r="R905" s="10"/>
     </row>
     <row r="906">
-      <c r="R906" s="8"/>
+      <c r="R906" s="10"/>
     </row>
     <row r="907">
-      <c r="R907" s="8"/>
+      <c r="R907" s="10"/>
     </row>
     <row r="908">
-      <c r="R908" s="8"/>
+      <c r="R908" s="10"/>
     </row>
     <row r="909">
-      <c r="R909" s="8"/>
+      <c r="R909" s="10"/>
     </row>
     <row r="910">
-      <c r="R910" s="8"/>
+      <c r="R910" s="10"/>
     </row>
     <row r="911">
-      <c r="R911" s="8"/>
+      <c r="R911" s="10"/>
     </row>
     <row r="912">
-      <c r="R912" s="8"/>
+      <c r="R912" s="10"/>
     </row>
     <row r="913">
-      <c r="R913" s="8"/>
+      <c r="R913" s="10"/>
     </row>
     <row r="914">
-      <c r="R914" s="8"/>
+      <c r="R914" s="10"/>
     </row>
     <row r="915">
-      <c r="R915" s="8"/>
+      <c r="R915" s="10"/>
     </row>
     <row r="916">
-      <c r="R916" s="8"/>
+      <c r="R916" s="10"/>
     </row>
     <row r="917">
-      <c r="R917" s="8"/>
+      <c r="R917" s="10"/>
     </row>
     <row r="918">
-      <c r="R918" s="8"/>
+      <c r="R918" s="10"/>
     </row>
     <row r="919">
-      <c r="R919" s="8"/>
+      <c r="R919" s="10"/>
     </row>
     <row r="920">
-      <c r="R920" s="8"/>
+      <c r="R920" s="10"/>
     </row>
     <row r="921">
-      <c r="R921" s="8"/>
+      <c r="R921" s="10"/>
     </row>
     <row r="922">
-      <c r="R922" s="8"/>
+      <c r="R922" s="10"/>
     </row>
     <row r="923">
-      <c r="R923" s="8"/>
+      <c r="R923" s="10"/>
     </row>
     <row r="924">
-      <c r="R924" s="8"/>
+      <c r="R924" s="10"/>
     </row>
     <row r="925">
-      <c r="R925" s="8"/>
+      <c r="R925" s="10"/>
     </row>
     <row r="926">
-      <c r="R926" s="8"/>
+      <c r="R926" s="10"/>
     </row>
     <row r="927">
-      <c r="R927" s="8"/>
+      <c r="R927" s="10"/>
     </row>
     <row r="928">
-      <c r="R928" s="8"/>
+      <c r="R928" s="10"/>
     </row>
     <row r="929">
-      <c r="R929" s="8"/>
+      <c r="R929" s="10"/>
     </row>
     <row r="930">
-      <c r="R930" s="8"/>
+      <c r="R930" s="10"/>
     </row>
     <row r="931">
-      <c r="R931" s="8"/>
+      <c r="R931" s="10"/>
     </row>
     <row r="932">
-      <c r="R932" s="8"/>
+      <c r="R932" s="10"/>
     </row>
     <row r="933">
-      <c r="R933" s="8"/>
+      <c r="R933" s="10"/>
     </row>
     <row r="934">
-      <c r="R934" s="8"/>
+      <c r="R934" s="10"/>
     </row>
     <row r="935">
-      <c r="R935" s="8"/>
+      <c r="R935" s="10"/>
     </row>
     <row r="936">
-      <c r="R936" s="8"/>
+      <c r="R936" s="10"/>
     </row>
     <row r="937">
-      <c r="R937" s="8"/>
+      <c r="R937" s="10"/>
     </row>
     <row r="938">
-      <c r="R938" s="8"/>
+      <c r="R938" s="10"/>
     </row>
     <row r="939">
-      <c r="R939" s="8"/>
+      <c r="R939" s="10"/>
     </row>
     <row r="940">
-      <c r="R940" s="8"/>
+      <c r="R940" s="10"/>
     </row>
     <row r="941">
-      <c r="R941" s="8"/>
+      <c r="R941" s="10"/>
     </row>
     <row r="942">
-      <c r="R942" s="8"/>
+      <c r="R942" s="10"/>
     </row>
     <row r="943">
-      <c r="R943" s="8"/>
+      <c r="R943" s="10"/>
     </row>
     <row r="944">
-      <c r="R944" s="8"/>
+      <c r="R944" s="10"/>
     </row>
     <row r="945">
-      <c r="R945" s="8"/>
+      <c r="R945" s="10"/>
     </row>
     <row r="946">
-      <c r="R946" s="8"/>
+      <c r="R946" s="10"/>
     </row>
     <row r="947">
-      <c r="R947" s="8"/>
+      <c r="R947" s="10"/>
     </row>
     <row r="948">
-      <c r="R948" s="8"/>
+      <c r="R948" s="10"/>
     </row>
     <row r="949">
-      <c r="R949" s="8"/>
+      <c r="R949" s="10"/>
     </row>
     <row r="950">
-      <c r="R950" s="8"/>
+      <c r="R950" s="10"/>
     </row>
     <row r="951">
-      <c r="R951" s="8"/>
+      <c r="R951" s="10"/>
     </row>
     <row r="952">
-      <c r="R952" s="8"/>
+      <c r="R952" s="10"/>
     </row>
     <row r="953">
-      <c r="R953" s="8"/>
+      <c r="R953" s="10"/>
     </row>
     <row r="954">
-      <c r="R954" s="8"/>
+      <c r="R954" s="10"/>
     </row>
     <row r="955">
-      <c r="R955" s="8"/>
+      <c r="R955" s="10"/>
     </row>
     <row r="956">
-      <c r="R956" s="8"/>
+      <c r="R956" s="10"/>
     </row>
     <row r="957">
-      <c r="R957" s="8"/>
+      <c r="R957" s="10"/>
     </row>
     <row r="958">
-      <c r="R958" s="8"/>
+      <c r="R958" s="10"/>
     </row>
     <row r="959">
-      <c r="R959" s="8"/>
+      <c r="R959" s="10"/>
     </row>
     <row r="960">
-      <c r="R960" s="8"/>
+      <c r="R960" s="10"/>
     </row>
     <row r="961">
-      <c r="R961" s="8"/>
+      <c r="R961" s="10"/>
     </row>
     <row r="962">
-      <c r="R962" s="8"/>
+      <c r="R962" s="10"/>
     </row>
     <row r="963">
-      <c r="R963" s="8"/>
+      <c r="R963" s="10"/>
     </row>
     <row r="964">
-      <c r="R964" s="8"/>
+      <c r="R964" s="10"/>
     </row>
     <row r="965">
-      <c r="R965" s="8"/>
+      <c r="R965" s="10"/>
     </row>
     <row r="966">
-      <c r="R966" s="8"/>
+      <c r="R966" s="10"/>
     </row>
     <row r="967">
-      <c r="R967" s="8"/>
+      <c r="R967" s="10"/>
     </row>
     <row r="968">
-      <c r="R968" s="8"/>
+      <c r="R968" s="10"/>
     </row>
     <row r="969">
-      <c r="R969" s="8"/>
+      <c r="R969" s="10"/>
     </row>
     <row r="970">
-      <c r="R970" s="8"/>
+      <c r="R970" s="10"/>
     </row>
     <row r="971">
-      <c r="R971" s="8"/>
+      <c r="R971" s="10"/>
     </row>
     <row r="972">
-      <c r="R972" s="8"/>
+      <c r="R972" s="10"/>
     </row>
     <row r="973">
-      <c r="R973" s="8"/>
+      <c r="R973" s="10"/>
     </row>
     <row r="974">
-      <c r="R974" s="8"/>
+      <c r="R974" s="10"/>
     </row>
     <row r="975">
-      <c r="R975" s="8"/>
+      <c r="R975" s="10"/>
     </row>
     <row r="976">
-      <c r="R976" s="8"/>
+      <c r="R976" s="10"/>
     </row>
     <row r="977">
-      <c r="R977" s="8"/>
+      <c r="R977" s="10"/>
     </row>
     <row r="978">
-      <c r="R978" s="8"/>
+      <c r="R978" s="10"/>
     </row>
     <row r="979">
-      <c r="R979" s="8"/>
+      <c r="R979" s="10"/>
     </row>
     <row r="980">
-      <c r="R980" s="8"/>
+      <c r="R980" s="10"/>
     </row>
     <row r="981">
-      <c r="R981" s="8"/>
+      <c r="R981" s="10"/>
     </row>
     <row r="982">
-      <c r="R982" s="8"/>
+      <c r="R982" s="10"/>
     </row>
     <row r="983">
-      <c r="R983" s="8"/>
+      <c r="R983" s="10"/>
     </row>
     <row r="984">
-      <c r="R984" s="8"/>
+      <c r="R984" s="10"/>
     </row>
     <row r="985">
-      <c r="R985" s="8"/>
+      <c r="R985" s="10"/>
     </row>
     <row r="986">
-      <c r="R986" s="8"/>
+      <c r="R986" s="10"/>
     </row>
     <row r="987">
-      <c r="R987" s="8"/>
+      <c r="R987" s="10"/>
     </row>
     <row r="988">
-      <c r="R988" s="8"/>
+      <c r="R988" s="10"/>
     </row>
     <row r="989">
-      <c r="R989" s="8"/>
+      <c r="R989" s="10"/>
     </row>
     <row r="990">
-      <c r="R990" s="8"/>
+      <c r="R990" s="10"/>
     </row>
     <row r="991">
-      <c r="R991" s="8"/>
+      <c r="R991" s="10"/>
     </row>
     <row r="992">
-      <c r="R992" s="8"/>
+      <c r="R992" s="10"/>
     </row>
     <row r="993">
-      <c r="R993" s="8"/>
+      <c r="R993" s="10"/>
     </row>
     <row r="994">
-      <c r="R994" s="8"/>
+      <c r="R994" s="10"/>
     </row>
     <row r="995">
-      <c r="R995" s="8"/>
+      <c r="R995" s="10"/>
     </row>
     <row r="996">
-      <c r="R996" s="8"/>
+      <c r="R996" s="10"/>
     </row>
     <row r="997">
-      <c r="R997" s="8"/>
+      <c r="R997" s="10"/>
     </row>
     <row r="998">
-      <c r="R998" s="8"/>
+      <c r="R998" s="10"/>
     </row>
     <row r="999">
-      <c r="R999" s="8"/>
-    </row>
-    <row r="1000">
-      <c r="R1000" s="8"/>
+      <c r="R999" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4011,173 +4017,173 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="4" t="str">
+      <c r="J2" s="5" t="str">
         <f>Main!M2</f>
         <v>USD 11.2</v>
       </c>
-      <c r="K2" s="12" t="str">
+      <c r="K2" s="14" t="str">
         <f>Main!N2</f>
         <v>USD 15</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="15">
         <v>30.0</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="4" t="str">
+      <c r="J3" s="5" t="str">
         <f>Main!M3</f>
         <v>USD 15</v>
       </c>
-      <c r="K3" s="4" t="str">
+      <c r="K3" s="5" t="str">
         <f>Main!N3</f>
         <v>USD 18</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="4">
         <v>50.0</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="4">
         <v>1.0</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="Q4" s="15"/>
+      <c r="Q4" s="17"/>
     </row>
     <row r="5">
-      <c r="D5" s="11"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6">
-      <c r="D6" s="11"/>
+      <c r="D6" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>